<commit_message>
DE data and figures (2005 obs.), xls
</commit_message>
<xml_diff>
--- a/questionnaires/board.xlsx
+++ b/questionnaires/board.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="843">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="847">
   <si>
     <t>Country</t>
   </si>
@@ -1286,9 +1286,6 @@
     <t>https://lse.eu.qualtrics.com/jfe/form/SV_02uibrdpLtSCOCW?Q_Language=JA</t>
   </si>
   <si>
-    <t>?Q_Language=ID</t>
-  </si>
-  <si>
     <t>?Q_Language=UK</t>
   </si>
   <si>
@@ -2174,9 +2171,6 @@
     <t>2.5 Agglomeration size</t>
   </si>
   <si>
-    <t>t</t>
-  </si>
-  <si>
     <t>2.6 Race/nationality</t>
   </si>
   <si>
@@ -2234,9 +2228,6 @@
     <t>14.9, 14.11 Change to "limit or renounce"</t>
   </si>
   <si>
-    <t>135, 136, 137 Adapt new question positive/costless</t>
-  </si>
-  <si>
     <t>16.7 Translate "Transfers from high-income countries"</t>
   </si>
   <si>
@@ -2553,6 +2544,27 @@
   </si>
   <si>
     <t>https://lse.eu.qualtrics.com/WRQualtricsControlPanel/File.php?F=F_9RF3ckVwWR9MH1Y</t>
+  </si>
+  <si>
+    <t>~ Adrien</t>
+  </si>
+  <si>
+    <t>~ Tarcilia</t>
+  </si>
+  <si>
+    <t>https://lse.eu.qualtrics.com/jfe/form/SV_73wzPC2ZxXEm0su?Q_Language=ID</t>
+  </si>
+  <si>
+    <t>https://lse.fra1.qualtrics.com/public-quotas?SID=SV_73wzPC2ZxXEm0su</t>
+  </si>
+  <si>
+    <t>135, 136, 137 Adapt new question positive/costless "class"</t>
+  </si>
+  <si>
+    <t>Pro Pemerintah (PDI Perjuangan / Golkar / PKB / NasDem / PPP / dsb)Oposisi (Gerindra / PKS / Partai Demokrat / PAN / dsb)</t>
+  </si>
+  <si>
+    <t>t, test</t>
   </si>
 </sst>
 </file>
@@ -2989,7 +3001,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3174,7 +3186,7 @@
         <v>28</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>28</v>
@@ -3186,18 +3198,20 @@
         <v>28</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="R3" s="3"/>
+      <c r="R3" s="3" t="s">
+        <v>841</v>
+      </c>
       <c r="S3" s="1" t="s">
         <v>28</v>
       </c>
@@ -3246,7 +3260,7 @@
         <v>28</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>28</v>
@@ -3309,10 +3323,13 @@
         <v>28</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>786</v>
+        <v>783</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>833</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="P5" s="3" t="s">
         <v>28</v>
@@ -3394,7 +3411,7 @@
         <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>35</v>
@@ -3403,26 +3420,28 @@
         <v>35</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>839</v>
-      </c>
-      <c r="J7" s="1"/>
+        <v>836</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>840</v>
+      </c>
       <c r="K7" s="1" t="s">
         <v>35</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>28</v>
@@ -4228,10 +4247,10 @@
       </c>
       <c r="L18" s="1"/>
       <c r="N18" s="1" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="P18" s="1"/>
       <c r="S18" t="s">
@@ -4350,7 +4369,7 @@
         <v>189</v>
       </c>
       <c r="N20" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="O20" t="s">
         <v>191</v>
@@ -4876,7 +4895,7 @@
         <v>228</v>
       </c>
       <c r="P28" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="Q28" t="s">
         <v>112</v>
@@ -5446,7 +5465,7 @@
         <v>290</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="O43" s="1" t="s">
         <v>291</v>
@@ -5455,10 +5474,10 @@
         <v>292</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="R43" s="1" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="S43" s="1" t="s">
         <v>293</v>
@@ -5645,7 +5664,7 @@
         <v>332</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="P46" s="1" t="s">
         <v>333</v>
@@ -5669,7 +5688,7 @@
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -7550,100 +7569,102 @@
         <v>419</v>
       </c>
       <c r="H71" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="I71" t="s">
-        <v>838</v>
-      </c>
-      <c r="J71" s="16" t="s">
+        <v>835</v>
+      </c>
+      <c r="J71" t="s">
+        <v>842</v>
+      </c>
+      <c r="K71" s="16" t="s">
+        <v>830</v>
+      </c>
+      <c r="L71" t="s">
+        <v>776</v>
+      </c>
+      <c r="M71" s="16" t="s">
+        <v>831</v>
+      </c>
+      <c r="N71" s="16" t="s">
         <v>420</v>
       </c>
-      <c r="K71" s="16" t="s">
-        <v>833</v>
-      </c>
-      <c r="L71" t="s">
-        <v>779</v>
-      </c>
-      <c r="M71" s="16" t="s">
-        <v>834</v>
-      </c>
-      <c r="N71" s="16" t="s">
+      <c r="O71" s="16" t="s">
         <v>421</v>
       </c>
-      <c r="O71" s="16" t="s">
+      <c r="P71" t="s">
         <v>422</v>
       </c>
-      <c r="P71" t="s">
+      <c r="Q71" t="s">
+        <v>820</v>
+      </c>
+      <c r="R71" t="s">
         <v>423</v>
       </c>
-      <c r="Q71" t="s">
-        <v>823</v>
-      </c>
-      <c r="R71" t="s">
+      <c r="S71" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="S71" s="16" t="s">
+      <c r="T71" s="20" t="s">
         <v>425</v>
       </c>
-      <c r="T71" s="20" t="s">
+      <c r="U71" s="16" t="s">
         <v>426</v>
       </c>
-      <c r="U71" s="16" t="s">
+      <c r="W71" t="s">
         <v>427</v>
       </c>
-      <c r="W71" t="s">
+      <c r="X71" t="s">
         <v>428</v>
       </c>
-      <c r="X71" t="s">
+      <c r="Y71" t="s">
         <v>429</v>
       </c>
-      <c r="Y71" t="s">
-        <v>430</v>
-      </c>
       <c r="Z71" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="B72" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="C72" t="s">
+        <v>811</v>
+      </c>
+      <c r="D72" t="s">
+        <v>812</v>
+      </c>
+      <c r="E72" t="s">
+        <v>810</v>
+      </c>
+      <c r="F72" t="s">
+        <v>813</v>
+      </c>
+      <c r="G72" t="s">
         <v>814</v>
       </c>
-      <c r="D72" t="s">
+      <c r="H72" t="s">
+        <v>778</v>
+      </c>
+      <c r="I72" t="s">
+        <v>823</v>
+      </c>
+      <c r="J72" t="s">
+        <v>843</v>
+      </c>
+      <c r="K72" t="s">
+        <v>775</v>
+      </c>
+      <c r="L72" t="s">
         <v>815</v>
-      </c>
-      <c r="E72" t="s">
-        <v>813</v>
-      </c>
-      <c r="F72" t="s">
-        <v>816</v>
-      </c>
-      <c r="G72" t="s">
-        <v>817</v>
-      </c>
-      <c r="H72" t="s">
-        <v>781</v>
-      </c>
-      <c r="I72" t="s">
-        <v>826</v>
-      </c>
-      <c r="J72" s="16"/>
-      <c r="K72" t="s">
-        <v>778</v>
-      </c>
-      <c r="L72" t="s">
-        <v>818</v>
       </c>
       <c r="M72" s="16"/>
       <c r="N72" s="16"/>
       <c r="O72" s="16"/>
       <c r="Q72" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="S72" s="16"/>
       <c r="T72" s="20"/>
@@ -7651,7 +7672,7 @@
     </row>
     <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B73">
         <v>0.37862000000000001</v>
@@ -7705,7 +7726,7 @@
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="S73" s="16" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="T73">
         <v>0.15443999999999999</v>
@@ -7725,7 +7746,7 @@
     </row>
     <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B74">
         <v>1.5</v>
@@ -7808,7 +7829,7 @@
     </row>
     <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B75">
         <v>1.804</v>
@@ -7861,7 +7882,7 @@
     </row>
     <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B76">
         <v>0.36799999999999999</v>
@@ -7914,7 +7935,7 @@
     </row>
     <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B77">
         <v>6.6000000000000003E-2</v>
@@ -7943,7 +7964,7 @@
     </row>
     <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B78">
         <v>0.90300000000000002</v>
@@ -7972,7 +7993,7 @@
     </row>
     <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D79">
         <f>240.49/D9</f>
@@ -7989,1254 +8010,1254 @@
     </row>
     <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B80" t="s">
         <v>439</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" t="s">
+        <v>439</v>
+      </c>
+      <c r="D80" t="s">
+        <v>439</v>
+      </c>
+      <c r="E80" t="s">
+        <v>439</v>
+      </c>
+      <c r="F80" t="s">
         <v>440</v>
       </c>
-      <c r="C80" t="s">
-        <v>440</v>
-      </c>
-      <c r="D80" t="s">
-        <v>440</v>
-      </c>
-      <c r="E80" t="s">
-        <v>440</v>
-      </c>
-      <c r="F80" t="s">
+      <c r="G80" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="G80" s="2" t="s">
+      <c r="H80" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="I80" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="H80" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="I80" s="2" t="s">
+      <c r="J80" t="s">
         <v>443</v>
       </c>
-      <c r="J80" t="s">
+      <c r="K80" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="K80" s="2" t="s">
+      <c r="L80" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="L80" s="2" t="s">
+      <c r="M80" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="M80" s="2" t="s">
+      <c r="N80" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="O80" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="N80" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="O80" s="2" t="s">
+      <c r="P80" t="s">
         <v>448</v>
       </c>
-      <c r="P80" t="s">
+      <c r="Q80" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="Q80" s="2" t="s">
+      <c r="R80" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="S80" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="R80" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="S80" s="2" t="s">
+      <c r="T80" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="T80" s="2" t="s">
+      <c r="U80" s="2" t="s">
         <v>452</v>
-      </c>
-      <c r="U80" s="2" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B81" t="s">
         <v>454</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" t="s">
         <v>455</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
         <v>456</v>
       </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>457</v>
       </c>
-      <c r="E81" t="s">
+      <c r="F81" t="s">
+        <v>454</v>
+      </c>
+      <c r="G81" t="s">
         <v>458</v>
       </c>
-      <c r="F81" t="s">
+      <c r="H81" t="s">
+        <v>459</v>
+      </c>
+      <c r="I81" t="s">
+        <v>460</v>
+      </c>
+      <c r="J81" t="s">
+        <v>461</v>
+      </c>
+      <c r="K81" t="s">
+        <v>462</v>
+      </c>
+      <c r="L81" t="s">
+        <v>463</v>
+      </c>
+      <c r="M81" t="s">
         <v>455</v>
       </c>
-      <c r="G81" t="s">
-        <v>459</v>
-      </c>
-      <c r="H81" t="s">
-        <v>460</v>
-      </c>
-      <c r="I81" t="s">
-        <v>461</v>
-      </c>
-      <c r="J81" t="s">
-        <v>462</v>
-      </c>
-      <c r="K81" t="s">
+      <c r="N81" t="s">
+        <v>454</v>
+      </c>
+      <c r="O81" t="s">
+        <v>464</v>
+      </c>
+      <c r="P81" t="s">
         <v>463</v>
       </c>
-      <c r="L81" t="s">
-        <v>464</v>
-      </c>
-      <c r="M81" t="s">
-        <v>456</v>
-      </c>
-      <c r="N81" t="s">
-        <v>455</v>
-      </c>
-      <c r="O81" t="s">
+      <c r="Q81" t="s">
+        <v>457</v>
+      </c>
+      <c r="R81" t="s">
+        <v>463</v>
+      </c>
+      <c r="S81" t="s">
+        <v>762</v>
+      </c>
+      <c r="T81" t="s">
         <v>465</v>
       </c>
-      <c r="P81" t="s">
-        <v>464</v>
-      </c>
-      <c r="Q81" t="s">
-        <v>458</v>
-      </c>
-      <c r="R81" t="s">
-        <v>464</v>
-      </c>
-      <c r="S81" t="s">
-        <v>765</v>
-      </c>
-      <c r="T81" t="s">
+      <c r="U81" t="s">
         <v>466</v>
-      </c>
-      <c r="U81" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="S82" t="s">
         <v>468</v>
       </c>
-      <c r="S82" t="s">
+      <c r="T82" t="s">
         <v>469</v>
       </c>
-      <c r="T82" t="s">
+      <c r="U82" t="s">
         <v>470</v>
-      </c>
-      <c r="U82" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="S83" s="7" t="s">
         <v>472</v>
-      </c>
-      <c r="S83" s="7" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B84" t="s">
         <v>474</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" t="s">
+        <v>474</v>
+      </c>
+      <c r="D84" t="s">
+        <v>474</v>
+      </c>
+      <c r="E84" t="s">
+        <v>474</v>
+      </c>
+      <c r="F84" t="s">
+        <v>474</v>
+      </c>
+      <c r="G84" t="s">
         <v>475</v>
       </c>
-      <c r="C84" t="s">
-        <v>475</v>
-      </c>
-      <c r="D84" t="s">
-        <v>475</v>
-      </c>
-      <c r="E84" t="s">
-        <v>475</v>
-      </c>
-      <c r="F84" t="s">
-        <v>475</v>
-      </c>
-      <c r="G84" t="s">
+      <c r="H84" t="s">
         <v>476</v>
       </c>
-      <c r="H84" t="s">
+      <c r="I84" t="s">
         <v>477</v>
       </c>
-      <c r="I84" t="s">
+      <c r="J84" t="s">
         <v>478</v>
       </c>
-      <c r="J84" t="s">
+      <c r="S84" t="s">
         <v>479</v>
       </c>
-      <c r="S84" t="s">
-        <v>480</v>
-      </c>
       <c r="T84" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="U84" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="I85" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="I85" s="2" t="s">
+      <c r="S85" t="s">
         <v>482</v>
       </c>
-      <c r="S85" t="s">
+      <c r="T85" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="T85" s="2" t="s">
+      <c r="U85" t="s">
         <v>484</v>
-      </c>
-      <c r="U85" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="F86" t="s">
         <v>486</v>
       </c>
-      <c r="F86" t="s">
+      <c r="I86" t="s">
         <v>487</v>
       </c>
-      <c r="I86" t="s">
+      <c r="S86" t="s">
         <v>488</v>
       </c>
-      <c r="S86" t="s">
+      <c r="T86" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="T86" s="2" t="s">
-        <v>490</v>
-      </c>
       <c r="U86" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="S87" t="s">
         <v>491</v>
-      </c>
-      <c r="S87" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="S88" s="21" t="s">
         <v>493</v>
-      </c>
-      <c r="S88" s="21" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="S89" t="s">
         <v>495</v>
-      </c>
-      <c r="S89" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="C90" t="s">
         <v>497</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D90" t="s">
         <v>498</v>
       </c>
-      <c r="D90" t="s">
+      <c r="E90" t="s">
         <v>499</v>
       </c>
-      <c r="E90" t="s">
+      <c r="F90" t="s">
         <v>500</v>
       </c>
-      <c r="F90" t="s">
+      <c r="G90" t="s">
         <v>501</v>
       </c>
-      <c r="G90" t="s">
+      <c r="H90" t="s">
         <v>502</v>
       </c>
-      <c r="H90" t="s">
+      <c r="I90" t="s">
         <v>503</v>
       </c>
-      <c r="I90" t="s">
+      <c r="J90" t="s">
         <v>504</v>
       </c>
-      <c r="J90" t="s">
+      <c r="K90" t="s">
         <v>505</v>
       </c>
-      <c r="K90" t="s">
+      <c r="L90" t="s">
         <v>506</v>
       </c>
-      <c r="L90" t="s">
+      <c r="M90" t="s">
         <v>507</v>
       </c>
-      <c r="M90" t="s">
+      <c r="N90" t="s">
         <v>508</v>
       </c>
-      <c r="N90" t="s">
+      <c r="O90" t="s">
         <v>509</v>
       </c>
-      <c r="O90" t="s">
+      <c r="P90" t="s">
         <v>510</v>
       </c>
-      <c r="P90" t="s">
+      <c r="Q90" t="s">
+        <v>512</v>
+      </c>
+      <c r="R90" t="s">
         <v>511</v>
       </c>
-      <c r="Q90" t="s">
+      <c r="S90" t="s">
         <v>513</v>
       </c>
-      <c r="R90" t="s">
-        <v>512</v>
-      </c>
-      <c r="S90" t="s">
+      <c r="T90" t="s">
         <v>514</v>
       </c>
-      <c r="T90" t="s">
+      <c r="U90" t="s">
         <v>515</v>
-      </c>
-      <c r="U90" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="C91" t="s">
         <v>517</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
         <v>518</v>
       </c>
-      <c r="D91" t="s">
+      <c r="E91" t="s">
         <v>519</v>
       </c>
-      <c r="E91" t="s">
+      <c r="F91" t="s">
         <v>520</v>
       </c>
-      <c r="F91" t="s">
+      <c r="G91" t="s">
         <v>521</v>
       </c>
-      <c r="G91" t="s">
+      <c r="H91" t="s">
         <v>522</v>
       </c>
-      <c r="H91" t="s">
+      <c r="I91" t="s">
         <v>523</v>
       </c>
-      <c r="I91" t="s">
+      <c r="J91" t="s">
         <v>524</v>
       </c>
-      <c r="J91" t="s">
+      <c r="K91" t="s">
         <v>525</v>
       </c>
-      <c r="K91" t="s">
+      <c r="L91" t="s">
         <v>526</v>
       </c>
-      <c r="L91" t="s">
+      <c r="M91" t="s">
         <v>527</v>
       </c>
-      <c r="M91" t="s">
+      <c r="N91" t="s">
         <v>528</v>
       </c>
-      <c r="N91" t="s">
+      <c r="O91" t="s">
         <v>529</v>
       </c>
-      <c r="O91" t="s">
+      <c r="P91" t="s">
         <v>530</v>
       </c>
-      <c r="P91" t="s">
+      <c r="Q91" t="s">
+        <v>532</v>
+      </c>
+      <c r="R91" t="s">
         <v>531</v>
       </c>
-      <c r="Q91" t="s">
+      <c r="S91" t="s">
         <v>533</v>
       </c>
-      <c r="R91" t="s">
-        <v>532</v>
-      </c>
-      <c r="S91" t="s">
+      <c r="T91" t="s">
         <v>534</v>
       </c>
-      <c r="T91" t="s">
+      <c r="U91" t="s">
         <v>535</v>
-      </c>
-      <c r="U91" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="C92" t="s">
         <v>537</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D92" t="s">
         <v>538</v>
       </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
         <v>539</v>
       </c>
-      <c r="E92" t="s">
+      <c r="F92" t="s">
         <v>540</v>
       </c>
-      <c r="F92" t="s">
+      <c r="G92" t="s">
         <v>541</v>
       </c>
-      <c r="G92" t="s">
+      <c r="H92" t="s">
         <v>542</v>
       </c>
-      <c r="H92" t="s">
+      <c r="I92" t="s">
         <v>543</v>
       </c>
-      <c r="I92" t="s">
+      <c r="J92" t="s">
         <v>544</v>
       </c>
-      <c r="J92" t="s">
+      <c r="K92" t="s">
         <v>545</v>
       </c>
-      <c r="K92" t="s">
+      <c r="L92" t="s">
         <v>546</v>
       </c>
-      <c r="L92" t="s">
+      <c r="M92" t="s">
         <v>547</v>
       </c>
-      <c r="M92" t="s">
+      <c r="N92" t="s">
         <v>548</v>
       </c>
-      <c r="N92" t="s">
+      <c r="O92" t="s">
         <v>549</v>
       </c>
-      <c r="O92" t="s">
+      <c r="P92" t="s">
+        <v>530</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>551</v>
+      </c>
+      <c r="R92" t="s">
         <v>550</v>
       </c>
-      <c r="P92" t="s">
-        <v>531</v>
-      </c>
-      <c r="Q92" t="s">
+      <c r="S92" t="s">
         <v>552</v>
       </c>
-      <c r="R92" t="s">
-        <v>551</v>
-      </c>
-      <c r="S92" t="s">
+      <c r="T92" t="s">
         <v>553</v>
       </c>
-      <c r="T92" t="s">
+      <c r="U92" t="s">
         <v>554</v>
-      </c>
-      <c r="U92" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="C93" t="s">
         <v>556</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
         <v>557</v>
       </c>
-      <c r="D93" t="s">
+      <c r="E93" t="s">
         <v>558</v>
       </c>
-      <c r="E93" t="s">
+      <c r="F93" t="s">
         <v>559</v>
       </c>
-      <c r="F93" t="s">
+      <c r="G93" t="s">
         <v>560</v>
       </c>
-      <c r="G93" t="s">
+      <c r="H93" t="s">
         <v>561</v>
       </c>
-      <c r="H93" t="s">
+      <c r="I93" t="s">
         <v>562</v>
       </c>
-      <c r="I93" t="s">
+      <c r="J93" t="s">
         <v>563</v>
       </c>
-      <c r="J93" t="s">
+      <c r="K93" t="s">
         <v>564</v>
       </c>
-      <c r="K93" t="s">
+      <c r="L93" t="s">
         <v>565</v>
       </c>
-      <c r="L93" t="s">
+      <c r="M93" t="s">
         <v>566</v>
       </c>
-      <c r="M93" t="s">
+      <c r="N93" t="s">
         <v>567</v>
       </c>
-      <c r="N93" t="s">
+      <c r="O93" t="s">
         <v>568</v>
       </c>
-      <c r="O93" t="s">
+      <c r="P93" t="s">
         <v>569</v>
       </c>
-      <c r="P93" t="s">
+      <c r="Q93" t="s">
+        <v>571</v>
+      </c>
+      <c r="R93" t="s">
         <v>570</v>
       </c>
-      <c r="Q93" t="s">
+      <c r="S93" s="22" t="s">
         <v>572</v>
       </c>
-      <c r="R93" t="s">
-        <v>571</v>
-      </c>
-      <c r="S93" s="22" t="s">
+      <c r="T93" t="s">
         <v>573</v>
       </c>
-      <c r="T93" t="s">
+      <c r="U93" t="s">
         <v>574</v>
-      </c>
-      <c r="U93" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="C94" t="s">
         <v>576</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D94" t="s">
         <v>577</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E94" t="s">
         <v>578</v>
       </c>
-      <c r="E94" t="s">
+      <c r="F94" t="s">
         <v>579</v>
       </c>
-      <c r="F94" t="s">
+      <c r="G94" t="s">
         <v>580</v>
       </c>
-      <c r="G94" t="s">
+      <c r="H94" t="s">
         <v>581</v>
       </c>
-      <c r="H94" t="s">
+      <c r="I94" t="s">
         <v>582</v>
       </c>
-      <c r="I94" t="s">
+      <c r="J94" t="s">
         <v>583</v>
       </c>
-      <c r="J94" t="s">
+      <c r="K94" t="s">
         <v>584</v>
       </c>
-      <c r="K94" t="s">
+      <c r="L94" t="s">
         <v>585</v>
       </c>
-      <c r="L94" t="s">
+      <c r="M94" t="s">
         <v>586</v>
       </c>
-      <c r="M94" t="s">
+      <c r="N94" t="s">
         <v>587</v>
       </c>
-      <c r="N94" t="s">
+      <c r="P94" t="s">
         <v>588</v>
       </c>
-      <c r="P94" t="s">
+      <c r="Q94" t="s">
+        <v>590</v>
+      </c>
+      <c r="R94" t="s">
         <v>589</v>
       </c>
-      <c r="Q94" t="s">
+      <c r="U94" t="s">
         <v>591</v>
-      </c>
-      <c r="R94" t="s">
-        <v>590</v>
-      </c>
-      <c r="U94" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="C95" t="s">
         <v>593</v>
       </c>
-      <c r="C95" t="s">
+      <c r="D95" t="s">
         <v>594</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
         <v>595</v>
       </c>
-      <c r="E95" t="s">
+      <c r="F95" t="s">
         <v>596</v>
       </c>
-      <c r="F95" t="s">
+      <c r="H95" t="s">
         <v>597</v>
       </c>
-      <c r="H95" t="s">
+      <c r="I95" t="s">
         <v>598</v>
       </c>
-      <c r="I95" t="s">
+      <c r="J95" t="s">
         <v>599</v>
       </c>
-      <c r="J95" t="s">
+      <c r="L95" t="s">
         <v>600</v>
       </c>
-      <c r="L95" t="s">
+      <c r="M95" t="s">
         <v>601</v>
       </c>
-      <c r="M95" t="s">
+      <c r="N95" t="s">
         <v>602</v>
       </c>
-      <c r="N95" t="s">
+      <c r="Q95" t="s">
         <v>603</v>
       </c>
-      <c r="Q95" t="s">
+      <c r="U95" t="s">
         <v>604</v>
-      </c>
-      <c r="U95" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="C96" t="s">
         <v>606</v>
       </c>
-      <c r="C96" t="s">
+      <c r="E96" t="s">
         <v>607</v>
       </c>
-      <c r="E96" t="s">
+      <c r="H96" t="s">
         <v>608</v>
       </c>
-      <c r="H96" t="s">
+      <c r="I96" t="s">
         <v>609</v>
       </c>
-      <c r="I96" t="s">
+      <c r="J96" t="s">
         <v>610</v>
       </c>
-      <c r="J96" t="s">
+      <c r="M96" t="s">
         <v>611</v>
       </c>
-      <c r="M96" t="s">
+      <c r="Q96" t="s">
         <v>612</v>
-      </c>
-      <c r="Q96" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="97" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="E97" t="s">
         <v>614</v>
       </c>
-      <c r="E97" t="s">
+      <c r="H97" t="s">
         <v>615</v>
       </c>
-      <c r="H97" t="s">
+      <c r="I97" t="s">
         <v>616</v>
       </c>
-      <c r="I97" t="s">
+      <c r="Q97" t="s">
         <v>617</v>
-      </c>
-      <c r="Q97" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="98" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="E98" t="s">
         <v>619</v>
       </c>
-      <c r="E98" t="s">
+      <c r="I98" t="s">
         <v>620</v>
-      </c>
-      <c r="I98" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="99" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="E99" t="s">
         <v>622</v>
       </c>
-      <c r="E99" t="s">
-        <v>623</v>
-      </c>
       <c r="I99" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="J99" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="100" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="S100" t="s">
         <v>624</v>
-      </c>
-      <c r="S100" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="101" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="S101" t="s">
         <v>626</v>
-      </c>
-      <c r="S101" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="102" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="S102" t="s">
         <v>628</v>
-      </c>
-      <c r="S102" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="103" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="B103" t="s">
         <v>630</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103" t="s">
+        <v>630</v>
+      </c>
+      <c r="D103" t="s">
+        <v>630</v>
+      </c>
+      <c r="E103" t="s">
+        <v>630</v>
+      </c>
+      <c r="F103" t="s">
+        <v>630</v>
+      </c>
+      <c r="G103" t="s">
+        <v>630</v>
+      </c>
+      <c r="I103" t="s">
+        <v>630</v>
+      </c>
+      <c r="J103" t="s">
+        <v>630</v>
+      </c>
+      <c r="K103" t="s">
+        <v>630</v>
+      </c>
+      <c r="N103" t="s">
         <v>631</v>
       </c>
-      <c r="C103" t="s">
-        <v>631</v>
-      </c>
-      <c r="D103" t="s">
-        <v>631</v>
-      </c>
-      <c r="E103" t="s">
-        <v>631</v>
-      </c>
-      <c r="F103" t="s">
-        <v>631</v>
-      </c>
-      <c r="G103" t="s">
-        <v>631</v>
-      </c>
-      <c r="I103" t="s">
-        <v>631</v>
-      </c>
-      <c r="J103" t="s">
-        <v>631</v>
-      </c>
-      <c r="K103" t="s">
-        <v>631</v>
-      </c>
-      <c r="N103" t="s">
+      <c r="S103" t="s">
         <v>632</v>
       </c>
-      <c r="S103" t="s">
-        <v>633</v>
-      </c>
       <c r="T103" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="U103" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="104" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
+        <v>633</v>
+      </c>
+      <c r="B104" t="s">
         <v>634</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C104" t="s">
+        <v>634</v>
+      </c>
+      <c r="D104" t="s">
+        <v>634</v>
+      </c>
+      <c r="E104" t="s">
+        <v>634</v>
+      </c>
+      <c r="F104" t="s">
+        <v>634</v>
+      </c>
+      <c r="G104" t="s">
+        <v>634</v>
+      </c>
+      <c r="H104" t="s">
+        <v>634</v>
+      </c>
+      <c r="I104" t="s">
+        <v>634</v>
+      </c>
+      <c r="J104" t="s">
+        <v>634</v>
+      </c>
+      <c r="K104" t="s">
+        <v>634</v>
+      </c>
+      <c r="L104" t="s">
+        <v>634</v>
+      </c>
+      <c r="R104" t="s">
+        <v>634</v>
+      </c>
+      <c r="S104" t="s">
         <v>635</v>
       </c>
-      <c r="C104" t="s">
-        <v>635</v>
-      </c>
-      <c r="D104" t="s">
-        <v>635</v>
-      </c>
-      <c r="E104" t="s">
-        <v>635</v>
-      </c>
-      <c r="F104" t="s">
-        <v>635</v>
-      </c>
-      <c r="G104" t="s">
-        <v>635</v>
-      </c>
-      <c r="H104" t="s">
-        <v>635</v>
-      </c>
-      <c r="I104" t="s">
-        <v>635</v>
-      </c>
-      <c r="J104" t="s">
-        <v>635</v>
-      </c>
-      <c r="K104" t="s">
-        <v>635</v>
-      </c>
-      <c r="L104" t="s">
-        <v>635</v>
-      </c>
-      <c r="R104" t="s">
-        <v>635</v>
-      </c>
-      <c r="S104" t="s">
-        <v>636</v>
-      </c>
       <c r="T104" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="U104" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="W104" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="105" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="B105" t="s">
         <v>637</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" t="s">
+        <v>637</v>
+      </c>
+      <c r="D105" t="s">
+        <v>637</v>
+      </c>
+      <c r="E105" t="s">
+        <v>637</v>
+      </c>
+      <c r="F105" t="s">
+        <v>637</v>
+      </c>
+      <c r="G105" t="s">
+        <v>637</v>
+      </c>
+      <c r="H105" t="s">
+        <v>637</v>
+      </c>
+      <c r="I105" t="s">
+        <v>637</v>
+      </c>
+      <c r="J105" t="s">
+        <v>637</v>
+      </c>
+      <c r="K105" t="s">
+        <v>637</v>
+      </c>
+      <c r="L105" t="s">
+        <v>637</v>
+      </c>
+      <c r="R105" t="s">
+        <v>637</v>
+      </c>
+      <c r="S105" t="s">
         <v>638</v>
       </c>
-      <c r="C105" t="s">
-        <v>638</v>
-      </c>
-      <c r="D105" t="s">
-        <v>638</v>
-      </c>
-      <c r="E105" t="s">
-        <v>638</v>
-      </c>
-      <c r="F105" t="s">
-        <v>638</v>
-      </c>
-      <c r="G105" t="s">
-        <v>638</v>
-      </c>
-      <c r="H105" t="s">
-        <v>638</v>
-      </c>
-      <c r="I105" t="s">
-        <v>638</v>
-      </c>
-      <c r="J105" t="s">
-        <v>638</v>
-      </c>
-      <c r="K105" t="s">
-        <v>638</v>
-      </c>
-      <c r="L105" t="s">
-        <v>638</v>
-      </c>
-      <c r="R105" t="s">
-        <v>638</v>
-      </c>
-      <c r="S105" t="s">
-        <v>639</v>
-      </c>
       <c r="T105" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="U105" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="W105" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="106" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
+        <v>639</v>
+      </c>
+      <c r="B106" t="s">
         <v>640</v>
       </c>
-      <c r="B106" t="s">
-        <v>641</v>
-      </c>
       <c r="C106" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D106" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E106" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="F106" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="T106" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="U106" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="W106" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="107" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
+        <v>641</v>
+      </c>
+      <c r="B107" t="s">
         <v>642</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
+        <v>642</v>
+      </c>
+      <c r="E107" t="s">
+        <v>642</v>
+      </c>
+      <c r="F107" t="s">
+        <v>642</v>
+      </c>
+      <c r="L107" t="s">
+        <v>642</v>
+      </c>
+      <c r="S107" t="s">
         <v>643</v>
       </c>
-      <c r="C107" t="s">
-        <v>643</v>
-      </c>
-      <c r="E107" t="s">
-        <v>643</v>
-      </c>
-      <c r="F107" t="s">
-        <v>643</v>
-      </c>
-      <c r="L107" t="s">
-        <v>643</v>
-      </c>
-      <c r="S107" t="s">
-        <v>644</v>
-      </c>
       <c r="T107" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="U107" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="W107" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="108" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
+        <v>644</v>
+      </c>
+      <c r="D108" t="s">
         <v>645</v>
       </c>
-      <c r="D108" t="s">
+      <c r="H108" t="s">
         <v>646</v>
       </c>
-      <c r="H108" t="s">
+      <c r="K108" t="s">
         <v>647</v>
-      </c>
-      <c r="K108" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="109" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="S109" t="s">
         <v>649</v>
       </c>
-      <c r="S109" t="s">
+      <c r="T109" t="s">
         <v>650</v>
       </c>
-      <c r="T109" t="s">
+      <c r="U109" t="s">
         <v>651</v>
-      </c>
-      <c r="U109" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="110" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="S110" t="s">
         <v>653</v>
       </c>
-      <c r="S110" t="s">
+      <c r="T110" t="s">
         <v>654</v>
       </c>
-      <c r="T110" t="s">
+      <c r="U110" t="s">
         <v>655</v>
-      </c>
-      <c r="U110" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="111" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="S111" t="s">
         <v>657</v>
       </c>
-      <c r="S111" t="s">
+      <c r="T111" t="s">
         <v>658</v>
       </c>
-      <c r="T111" t="s">
+      <c r="U111" t="s">
         <v>659</v>
-      </c>
-      <c r="U111" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="112" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="U112" t="s">
         <v>661</v>
-      </c>
-      <c r="U112" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="113" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="S113" t="s">
         <v>663</v>
-      </c>
-      <c r="S113" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="114" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="S114" t="s">
         <v>665</v>
       </c>
-      <c r="S114" t="s">
+      <c r="T114" s="23" t="s">
         <v>666</v>
       </c>
-      <c r="T114" s="23" t="s">
+      <c r="U114" t="s">
         <v>667</v>
-      </c>
-      <c r="U114" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="115" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
+        <v>668</v>
+      </c>
+      <c r="S115" t="s">
         <v>669</v>
-      </c>
-      <c r="S115" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="116" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
+        <v>670</v>
+      </c>
+      <c r="U116" t="s">
         <v>671</v>
-      </c>
-      <c r="U116" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="117" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="B117" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="C117" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="D117" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="E117" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="F117" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="G117" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="H117" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="I117" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="K117" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="L117" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="M117" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="P117" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="Q117" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="S117" t="s">
+        <v>707</v>
+      </c>
+      <c r="T117" t="s">
         <v>708</v>
       </c>
-      <c r="T117" t="s">
+      <c r="U117" t="s">
         <v>709</v>
-      </c>
-      <c r="U117" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="118" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="B118" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="C118" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="D118" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="E118" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="F118" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="G118" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="H118" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="I118" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="K118" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="L118" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="M118" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="P118" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="Q118" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="S118" t="s">
+        <v>703</v>
+      </c>
+      <c r="T118" t="s">
         <v>704</v>
       </c>
-      <c r="T118" t="s">
+      <c r="U118" t="s">
         <v>705</v>
-      </c>
-      <c r="U118" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="119" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
+        <v>752</v>
+      </c>
+      <c r="B119" s="9" t="s">
+        <v>761</v>
+      </c>
+      <c r="C119" s="9" t="s">
+        <v>760</v>
+      </c>
+      <c r="D119" t="s">
+        <v>759</v>
+      </c>
+      <c r="H119" s="9" t="s">
+        <v>758</v>
+      </c>
+      <c r="I119" t="s">
+        <v>757</v>
+      </c>
+      <c r="L119" s="9" t="s">
+        <v>756</v>
+      </c>
+      <c r="N119" s="9" t="s">
         <v>755</v>
       </c>
-      <c r="B119" s="9" t="s">
-        <v>764</v>
-      </c>
-      <c r="C119" s="9" t="s">
-        <v>763</v>
-      </c>
-      <c r="D119" t="s">
-        <v>762</v>
-      </c>
-      <c r="H119" s="9" t="s">
-        <v>761</v>
-      </c>
-      <c r="I119" t="s">
-        <v>760</v>
-      </c>
-      <c r="L119" s="9" t="s">
-        <v>759</v>
-      </c>
-      <c r="N119" s="9" t="s">
-        <v>758</v>
-      </c>
       <c r="O119" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="P119" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
     </row>
     <row r="120" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="B120" t="s">
         <v>673</v>
       </c>
-      <c r="B120" t="s">
+      <c r="C120" t="s">
         <v>674</v>
       </c>
-      <c r="C120" t="s">
+      <c r="D120" t="s">
         <v>675</v>
       </c>
-      <c r="D120" t="s">
+      <c r="E120" t="s">
         <v>676</v>
       </c>
-      <c r="E120" t="s">
+      <c r="F120" t="s">
         <v>677</v>
       </c>
-      <c r="F120" t="s">
+      <c r="G120" t="s">
         <v>678</v>
       </c>
-      <c r="G120" t="s">
+      <c r="I120" t="s">
         <v>679</v>
       </c>
-      <c r="I120" t="s">
+      <c r="J120" t="s">
         <v>680</v>
       </c>
-      <c r="J120" t="s">
+      <c r="K120" s="24" t="s">
         <v>681</v>
       </c>
-      <c r="K120" s="24" t="s">
+      <c r="L120" t="s">
+        <v>769</v>
+      </c>
+      <c r="M120" t="s">
+        <v>773</v>
+      </c>
+      <c r="N120" t="s">
+        <v>782</v>
+      </c>
+      <c r="O120" t="s">
+        <v>765</v>
+      </c>
+      <c r="P120" t="s">
+        <v>771</v>
+      </c>
+      <c r="S120" t="s">
         <v>682</v>
       </c>
-      <c r="L120" t="s">
-        <v>772</v>
-      </c>
-      <c r="M120" t="s">
-        <v>776</v>
-      </c>
-      <c r="N120" t="s">
-        <v>785</v>
-      </c>
-      <c r="O120" t="s">
-        <v>768</v>
-      </c>
-      <c r="P120" t="s">
-        <v>774</v>
-      </c>
-      <c r="S120" t="s">
+      <c r="T120" t="s">
         <v>683</v>
       </c>
-      <c r="T120" t="s">
+      <c r="U120" t="s">
         <v>684</v>
-      </c>
-      <c r="U120" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="121" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="C121" t="s">
         <v>686</v>
       </c>
-      <c r="C121" t="s">
+      <c r="D121" t="s">
+        <v>764</v>
+      </c>
+      <c r="E121" t="s">
         <v>687</v>
       </c>
-      <c r="D121" t="s">
-        <v>767</v>
-      </c>
-      <c r="E121" t="s">
+      <c r="G121" t="s">
         <v>688</v>
       </c>
-      <c r="G121" t="s">
+      <c r="H121" t="s">
         <v>689</v>
       </c>
-      <c r="H121" t="s">
+      <c r="I121" t="s">
         <v>690</v>
       </c>
-      <c r="I121" t="s">
+      <c r="J121" t="s">
         <v>691</v>
       </c>
-      <c r="J121" t="s">
+      <c r="K121" t="s">
         <v>692</v>
       </c>
-      <c r="K121" t="s">
+      <c r="N121" t="s">
         <v>693</v>
       </c>
-      <c r="N121" t="s">
+      <c r="O121" t="s">
         <v>694</v>
       </c>
-      <c r="O121" t="s">
+      <c r="P121" t="s">
+        <v>770</v>
+      </c>
+      <c r="R121" t="s">
         <v>695</v>
       </c>
-      <c r="P121" t="s">
-        <v>773</v>
-      </c>
-      <c r="R121" t="s">
+      <c r="T121" t="s">
         <v>696</v>
-      </c>
-      <c r="T121" t="s">
-        <v>697</v>
       </c>
     </row>
     <row r="122" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="S122" t="s">
         <v>698</v>
-      </c>
-      <c r="S122" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="123" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B123">
         <v>7</v>
@@ -9265,7 +9286,7 @@
     </row>
     <row r="124" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B124">
         <v>6300</v>
@@ -9297,7 +9318,7 @@
     </row>
     <row r="125" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B125">
         <v>6500</v>
@@ -9359,35 +9380,35 @@
     </row>
     <row r="126" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
+        <v>702</v>
+      </c>
+      <c r="S126" t="s">
         <v>703</v>
       </c>
-      <c r="S126" t="s">
+      <c r="T126" t="s">
         <v>704</v>
       </c>
-      <c r="T126" t="s">
+      <c r="U126" t="s">
         <v>705</v>
-      </c>
-      <c r="U126" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="127" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
+        <v>706</v>
+      </c>
+      <c r="S127" t="s">
         <v>707</v>
       </c>
-      <c r="S127" t="s">
+      <c r="T127" t="s">
         <v>708</v>
       </c>
-      <c r="T127" t="s">
+      <c r="U127" t="s">
         <v>709</v>
-      </c>
-      <c r="U127" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B129" t="s">
         <v>28</v>
@@ -9422,7 +9443,7 @@
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B130" t="s">
         <v>28</v>
@@ -9439,145 +9460,136 @@
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="E131" t="s">
+        <v>816</v>
+      </c>
+      <c r="I131" t="s">
         <v>713</v>
       </c>
-      <c r="E131" t="s">
-        <v>819</v>
-      </c>
-      <c r="I131" t="s">
-        <v>714</v>
-      </c>
       <c r="J131" t="s">
-        <v>714</v>
+        <v>846</v>
       </c>
       <c r="L131" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="M131" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="N131" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="O131" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="P131" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="Q131" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="R131" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="H132" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="N132" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="O132" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B133" t="s">
-        <v>714</v>
-      </c>
-      <c r="J133" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="134" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="135" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>719</v>
-      </c>
-      <c r="J135" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="M135" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="N135" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="O135" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="P135" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="R135" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="N136" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="O136" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="P136" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="R136" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="J137" t="s">
-        <v>714</v>
+        <v>845</v>
       </c>
       <c r="N137" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="O137" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="P137" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="R137" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="138" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="139" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>723</v>
-      </c>
-      <c r="J139" t="s">
-        <v>714</v>
+        <v>721</v>
       </c>
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="B140" t="s">
         <v>43</v>
@@ -9609,7 +9621,7 @@
     </row>
     <row r="141" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="B141" t="s">
         <v>43</v>
@@ -9638,306 +9650,274 @@
     </row>
     <row r="142" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>726</v>
-      </c>
-      <c r="J142" t="s">
-        <v>714</v>
+        <v>724</v>
       </c>
       <c r="R142" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="143" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="144" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>728</v>
-      </c>
-      <c r="J144" t="s">
-        <v>714</v>
+        <v>726</v>
       </c>
       <c r="N144" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="O144" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="P144" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="R144" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="N145" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="O145" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="P145" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="R145" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="146" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="147" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="148" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>732</v>
-      </c>
-      <c r="J148" t="s">
-        <v>714</v>
+        <v>730</v>
       </c>
     </row>
     <row r="149" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>828</v>
-      </c>
-      <c r="J149" t="s">
-        <v>714</v>
+        <v>825</v>
       </c>
       <c r="N149" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="O149" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="P149" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="150" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>734</v>
-      </c>
-      <c r="J150" t="s">
-        <v>716</v>
+        <v>732</v>
       </c>
     </row>
     <row r="151" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
-        <v>735</v>
-      </c>
-      <c r="J151" t="s">
-        <v>716</v>
+        <v>733</v>
       </c>
     </row>
     <row r="152" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
-        <v>736</v>
-      </c>
-      <c r="J152" t="s">
-        <v>714</v>
+        <v>844</v>
       </c>
       <c r="N152" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="O152" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="P152" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="153" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
     </row>
     <row r="154" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="N154" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="O154" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="P154" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
     </row>
     <row r="155" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
     </row>
     <row r="156" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>740</v>
-      </c>
-      <c r="J156" t="s">
-        <v>714</v>
+        <v>737</v>
       </c>
       <c r="N156" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="O156" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="P156" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="R156" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="157" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="N157" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="O157" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="P157" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="R157" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="158" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="I158" t="s">
         <v>43</v>
       </c>
-      <c r="J158" t="s">
-        <v>714</v>
-      </c>
       <c r="K158" t="s">
         <v>43</v>
       </c>
       <c r="N158" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="O158" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="P158" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="R158" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="159" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="N159" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="O159" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="P159" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="R159" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="161" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="162" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="163" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="H163" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="164" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="G164" s="1"/>
       <c r="H164" s="1"/>
       <c r="I164" s="1"/>
-      <c r="J164" s="1" t="s">
-        <v>733</v>
-      </c>
+      <c r="J164" s="1"/>
       <c r="O164" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="165" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
     </row>
     <row r="166" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="I166" s="1"/>
       <c r="K166" s="1"/>
     </row>
     <row r="167" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="B167" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
     </row>
     <row r="168" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="I168" s="1"/>
-      <c r="J168" t="s">
-        <v>716</v>
-      </c>
     </row>
     <row r="169" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
     </row>
     <row r="170" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="D170" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
     </row>
     <row r="171" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add electricity / gas prices
</commit_message>
<xml_diff>
--- a/questionnaires/board.xlsx
+++ b/questionnaires/board.xlsx
@@ -1,30 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afabre\Documents\www\oecd_climate\questionnaires\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474AFD58-0BD9-D840-A4BB-9AF3255CFE25}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7640"/>
+    <workbookView xWindow="-1840" yWindow="-19440" windowWidth="27260" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="846">
   <si>
     <t>Country</t>
   </si>
@@ -1325,18 +1332,12 @@
     <t>vid_cli M people permanently flooded in 2100 K17 RCP8.5 (Kulp &amp; Strauss, 2019 https://www.nature.com/articles/s41467-019-12808-z)</t>
   </si>
   <si>
-    <t>Price gasoline (05-Jul-2021) USD/Liter (Gallon for US)</t>
-  </si>
-  <si>
     <t>Price electricity for households (December-2020) USD/kWh</t>
   </si>
   <si>
     <t>Price natural gas for households (March-2021) USD/kWh</t>
   </si>
   <si>
-    <t>Price heating oil (05-Jul-2021) USD/Liter</t>
-  </si>
-  <si>
     <t>Price coal (bituminous) USD/t</t>
   </si>
   <si>
@@ -2562,12 +2563,18 @@
   </si>
   <si>
     <t>FR: Jérôme Pilette, 200$ / EN: Davenport</t>
+  </si>
+  <si>
+    <t>Price gasoline (05-Jul-2021 or 06-Sep-2021) USD/Liter (Gallon for US)</t>
+  </si>
+  <si>
+    <t>Price heating oil (05-Jul-2021 or 06-Sep-2021) USD/Liter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -2993,20 +3000,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P7" sqref="P7"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC78" sqref="AC78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3059,7 +3066,7 @@
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>18</v>
@@ -3092,7 +3099,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -3158,7 +3165,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
@@ -3196,19 +3203,19 @@
         <v>28</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="R3" s="3"/>
       <c r="S3" s="1" t="s">
@@ -3224,7 +3231,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
@@ -3259,7 +3266,7 @@
         <v>32</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>28</v>
@@ -3288,7 +3295,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -3323,7 +3330,7 @@
         <v>32</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>28</v>
@@ -3350,7 +3357,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -3415,7 +3422,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -3423,7 +3430,7 @@
         <v>35</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>35</v>
@@ -3432,28 +3439,28 @@
         <v>35</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>35</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>832</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>834</v>
-      </c>
       <c r="P7" s="3" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>28</v>
@@ -3468,7 +3475,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -3533,7 +3540,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>50</v>
       </c>
@@ -3616,7 +3623,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
@@ -3700,7 +3707,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>76</v>
       </c>
@@ -3783,7 +3790,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>102</v>
       </c>
@@ -3866,7 +3873,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>125</v>
       </c>
@@ -3949,7 +3956,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>138</v>
       </c>
@@ -4032,7 +4039,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>146</v>
       </c>
@@ -4097,7 +4104,7 @@
         <v>16942</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>149</v>
       </c>
@@ -4162,7 +4169,7 @@
         <v>23515</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>152</v>
       </c>
@@ -4227,7 +4234,7 @@
         <v>31800</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>155</v>
       </c>
@@ -4260,10 +4267,10 @@
       </c>
       <c r="K18" s="1"/>
       <c r="M18" s="1" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="O18" s="1"/>
       <c r="S18" t="s">
@@ -4279,7 +4286,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
@@ -4344,7 +4351,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>182</v>
       </c>
@@ -4382,7 +4389,7 @@
         <v>189</v>
       </c>
       <c r="M20" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="N20" t="s">
         <v>191</v>
@@ -4409,7 +4416,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>193</v>
       </c>
@@ -4474,7 +4481,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>206</v>
       </c>
@@ -4539,7 +4546,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>207</v>
       </c>
@@ -4604,7 +4611,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>208</v>
       </c>
@@ -4669,7 +4676,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>209</v>
       </c>
@@ -4734,7 +4741,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>210</v>
       </c>
@@ -4799,7 +4806,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>213</v>
       </c>
@@ -4864,7 +4871,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>222</v>
       </c>
@@ -4908,7 +4915,7 @@
         <v>228</v>
       </c>
       <c r="O28" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="P28" t="s">
         <v>112</v>
@@ -4929,7 +4936,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>230</v>
       </c>
@@ -4994,7 +5001,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>237</v>
       </c>
@@ -5038,7 +5045,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>249</v>
       </c>
@@ -5046,7 +5053,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>250</v>
       </c>
@@ -5111,7 +5118,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>253</v>
       </c>
@@ -5176,7 +5183,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>254</v>
       </c>
@@ -5241,7 +5248,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>255</v>
       </c>
@@ -5306,7 +5313,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>256</v>
       </c>
@@ -5371,7 +5378,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>259</v>
       </c>
@@ -5385,7 +5392,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>263</v>
       </c>
@@ -5399,7 +5406,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>267</v>
       </c>
@@ -5413,7 +5420,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>271</v>
       </c>
@@ -5421,7 +5428,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>273</v>
       </c>
@@ -5429,7 +5436,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>275</v>
       </c>
@@ -5440,7 +5447,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>278</v>
       </c>
@@ -5478,7 +5485,7 @@
         <v>290</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="N43" s="1" t="s">
         <v>291</v>
@@ -5487,10 +5494,10 @@
         <v>292</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="R43" s="1"/>
       <c r="S43" s="1" t="s">
@@ -5506,7 +5513,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>296</v>
       </c>
@@ -5571,7 +5578,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>300</v>
       </c>
@@ -5638,7 +5645,7 @@
       </c>
       <c r="X45" s="1"/>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>319</v>
       </c>
@@ -5679,7 +5686,7 @@
         <v>332</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="O46" s="1" t="s">
         <v>333</v>
@@ -5705,9 +5712,9 @@
       </c>
       <c r="X46" s="1"/>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -5740,7 +5747,7 @@
       <c r="V47" s="1"/>
       <c r="X47" s="1"/>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>339</v>
       </c>
@@ -5763,7 +5770,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>342</v>
       </c>
@@ -5827,7 +5834,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>355</v>
       </c>
@@ -5911,7 +5918,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>357</v>
       </c>
@@ -6019,7 +6026,7 @@
         <v>27.6</v>
       </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>358</v>
       </c>
@@ -6102,7 +6109,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>359</v>
       </c>
@@ -6208,7 +6215,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>361</v>
       </c>
@@ -6240,7 +6247,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>365</v>
       </c>
@@ -6323,7 +6330,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>373</v>
       </c>
@@ -6389,7 +6396,7 @@
       </c>
       <c r="Y56" s="2"/>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>374</v>
       </c>
@@ -6473,7 +6480,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>375</v>
       </c>
@@ -6583,7 +6590,7 @@
         <v>5.2325581395348841</v>
       </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>376</v>
       </c>
@@ -6667,7 +6674,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>377</v>
       </c>
@@ -6751,7 +6758,7 @@
         <v>39.738</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>378</v>
       </c>
@@ -6834,7 +6841,7 @@
         <v>7115854.8000000007</v>
       </c>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>379</v>
       </c>
@@ -6917,7 +6924,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>380</v>
       </c>
@@ -7027,7 +7034,7 @@
         <v>0.1125</v>
       </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>381</v>
       </c>
@@ -7137,7 +7144,7 @@
         <v>0.10350000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>382</v>
       </c>
@@ -7247,7 +7254,7 @@
         <v>147.96508326729767</v>
       </c>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>383</v>
       </c>
@@ -7291,7 +7298,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>386</v>
       </c>
@@ -7374,7 +7381,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>391</v>
       </c>
@@ -7458,7 +7465,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>395</v>
       </c>
@@ -7515,7 +7522,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>404</v>
       </c>
@@ -7581,7 +7588,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>413</v>
       </c>
@@ -7601,22 +7608,22 @@
         <v>419</v>
       </c>
       <c r="G71" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="H71" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="I71" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="J71" s="16" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="K71" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="L71" s="16" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="M71" s="16" t="s">
         <v>420</v>
@@ -7628,7 +7635,7 @@
         <v>422</v>
       </c>
       <c r="P71" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="Q71" t="s">
         <v>423</v>
@@ -7658,54 +7665,54 @@
         <v>427</v>
       </c>
     </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="B72" t="s">
+        <v>807</v>
+      </c>
+      <c r="C72" t="s">
+        <v>808</v>
+      </c>
+      <c r="D72" t="s">
+        <v>806</v>
+      </c>
+      <c r="E72" t="s">
         <v>809</v>
       </c>
-      <c r="C72" t="s">
+      <c r="F72" t="s">
         <v>810</v>
       </c>
-      <c r="D72" t="s">
-        <v>808</v>
-      </c>
-      <c r="E72" t="s">
+      <c r="G72" t="s">
+        <v>774</v>
+      </c>
+      <c r="H72" t="s">
+        <v>819</v>
+      </c>
+      <c r="I72" t="s">
+        <v>837</v>
+      </c>
+      <c r="J72" t="s">
+        <v>771</v>
+      </c>
+      <c r="K72" t="s">
         <v>811</v>
-      </c>
-      <c r="F72" t="s">
-        <v>812</v>
-      </c>
-      <c r="G72" t="s">
-        <v>776</v>
-      </c>
-      <c r="H72" t="s">
-        <v>821</v>
-      </c>
-      <c r="I72" t="s">
-        <v>839</v>
-      </c>
-      <c r="J72" t="s">
-        <v>773</v>
-      </c>
-      <c r="K72" t="s">
-        <v>813</v>
       </c>
       <c r="L72" s="16"/>
       <c r="M72" s="16"/>
       <c r="N72" s="16"/>
       <c r="P72" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="S72" s="16"/>
       <c r="T72" s="20"/>
       <c r="U72" s="16"/>
       <c r="V72" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.35">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="73" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>430</v>
       </c>
@@ -7779,7 +7786,7 @@
         <v>1.1820000000000001E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>432</v>
       </c>
@@ -7862,9 +7869,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>433</v>
+        <v>844</v>
       </c>
       <c r="B75">
         <v>1.9419999999999999</v>
@@ -7896,9 +7903,27 @@
       <c r="K75">
         <v>1.1140000000000001</v>
       </c>
+      <c r="L75">
+        <v>1.2470000000000001</v>
+      </c>
+      <c r="M75">
+        <v>1.1180000000000001</v>
+      </c>
+      <c r="N75">
+        <v>1.446</v>
+      </c>
+      <c r="O75">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="P75">
+        <v>1.0940000000000001</v>
+      </c>
       <c r="Q75">
         <v>1.1180000000000001</v>
       </c>
+      <c r="R75">
+        <v>2.0190000000000001</v>
+      </c>
       <c r="S75">
         <v>3.4790000000000001</v>
       </c>
@@ -7911,13 +7936,28 @@
       <c r="V75">
         <v>1.804</v>
       </c>
+      <c r="W75">
+        <v>0.40400000000000003</v>
+      </c>
       <c r="X75">
         <v>0.90300000000000002</v>
       </c>
-    </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="Y75">
+        <v>0.06</v>
+      </c>
+      <c r="Z75">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="AA75">
+        <v>0.621</v>
+      </c>
+      <c r="AB75">
+        <v>1.7490000000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B76">
         <v>0.26400000000000001</v>
@@ -7949,9 +7989,27 @@
       <c r="K76">
         <v>8.3000000000000004E-2</v>
       </c>
+      <c r="L76">
+        <v>0.111</v>
+      </c>
+      <c r="M76">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="N76">
+        <v>0.111</v>
+      </c>
+      <c r="O76">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="P76">
+        <v>0.22700000000000001</v>
+      </c>
       <c r="Q76">
         <v>0.13700000000000001</v>
       </c>
+      <c r="R76">
+        <v>0.17499999999999999</v>
+      </c>
       <c r="S76">
         <v>0.14799999999999999</v>
       </c>
@@ -7964,13 +8022,28 @@
       <c r="V76">
         <v>0.36799999999999999</v>
       </c>
+      <c r="W76">
+        <v>5.8999999999999997E-2</v>
+      </c>
       <c r="X76">
         <v>7.9000000000000001E-2</v>
       </c>
-    </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="Y76">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="Z76">
+        <v>6.2E-2</v>
+      </c>
+      <c r="AA76">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="AB76">
+        <v>0.22700000000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B77">
         <v>9.7000000000000003E-2</v>
@@ -7984,6 +8057,18 @@
       <c r="K77">
         <v>3.5000000000000003E-2</v>
       </c>
+      <c r="L77">
+        <v>2.7E-2</v>
+      </c>
+      <c r="M77">
+        <v>1.9E-2</v>
+      </c>
+      <c r="O77">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="P77">
+        <v>7.3999999999999996E-2</v>
+      </c>
       <c r="T77">
         <v>0.106</v>
       </c>
@@ -7996,10 +8081,16 @@
       <c r="X77">
         <v>1.7000000000000001E-2</v>
       </c>
-    </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="Z77">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AB77">
+        <v>7.0999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>436</v>
+        <v>845</v>
       </c>
       <c r="B78">
         <v>1.5329999999999999</v>
@@ -8013,6 +8104,12 @@
       <c r="E78">
         <v>0.81</v>
       </c>
+      <c r="L78">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="O78">
+        <v>0.755</v>
+      </c>
       <c r="T78">
         <v>1.754</v>
       </c>
@@ -8026,9 +8123,9 @@
         <v>0.81299999999999994</v>
       </c>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C79">
         <f>240.49/C9</f>
@@ -8043,861 +8140,942 @@
         <v>72.200772200772207</v>
       </c>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B80" t="s">
+        <v>437</v>
+      </c>
+      <c r="C80" t="s">
+        <v>437</v>
+      </c>
+      <c r="D80" t="s">
+        <v>437</v>
+      </c>
+      <c r="E80" t="s">
         <v>438</v>
       </c>
-      <c r="B80" t="s">
+      <c r="F80" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="C80" t="s">
+      <c r="G80" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="D80" t="s">
-        <v>439</v>
-      </c>
-      <c r="E80" t="s">
+      <c r="H80" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="F80" s="2" t="s">
+      <c r="I80" t="s">
         <v>441</v>
       </c>
-      <c r="G80" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="H80" s="2" t="s">
+      <c r="J80" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="I80" t="s">
+      <c r="K80" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="J80" s="2" t="s">
+      <c r="L80" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="K80" s="2" t="s">
+      <c r="M80" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="N80" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="L80" s="2" t="s">
+      <c r="O80" t="s">
         <v>446</v>
       </c>
-      <c r="M80" s="2" t="s">
+      <c r="P80" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="Q80" s="2" t="s">
         <v>445</v>
-      </c>
-      <c r="N80" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="O80" t="s">
-        <v>448</v>
-      </c>
-      <c r="P80" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="Q80" s="2" t="s">
-        <v>447</v>
       </c>
       <c r="R80" s="2"/>
       <c r="S80" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="T80" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="U80" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="T80" s="2" t="s">
+      <c r="V80" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="81" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="U80" s="2" t="s">
+      <c r="B81" t="s">
+        <v>453</v>
+      </c>
+      <c r="C81" t="s">
+        <v>454</v>
+      </c>
+      <c r="D81" t="s">
+        <v>455</v>
+      </c>
+      <c r="E81" t="s">
         <v>452</v>
       </c>
-      <c r="V80" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A81" s="1" t="s">
+      <c r="F81" t="s">
+        <v>456</v>
+      </c>
+      <c r="G81" t="s">
+        <v>457</v>
+      </c>
+      <c r="H81" t="s">
+        <v>458</v>
+      </c>
+      <c r="I81" t="s">
+        <v>459</v>
+      </c>
+      <c r="J81" t="s">
+        <v>460</v>
+      </c>
+      <c r="K81" t="s">
+        <v>461</v>
+      </c>
+      <c r="L81" t="s">
         <v>453</v>
       </c>
-      <c r="B81" t="s">
+      <c r="M81" t="s">
+        <v>452</v>
+      </c>
+      <c r="N81" t="s">
+        <v>462</v>
+      </c>
+      <c r="O81" t="s">
+        <v>461</v>
+      </c>
+      <c r="P81" t="s">
         <v>455</v>
       </c>
-      <c r="C81" t="s">
-        <v>456</v>
-      </c>
-      <c r="D81" t="s">
-        <v>457</v>
-      </c>
-      <c r="E81" t="s">
-        <v>454</v>
-      </c>
-      <c r="F81" t="s">
-        <v>458</v>
-      </c>
-      <c r="G81" t="s">
-        <v>459</v>
-      </c>
-      <c r="H81" t="s">
-        <v>460</v>
-      </c>
-      <c r="I81" t="s">
+      <c r="Q81" t="s">
         <v>461</v>
       </c>
-      <c r="J81" t="s">
-        <v>462</v>
-      </c>
-      <c r="K81" t="s">
+      <c r="S81" t="s">
+        <v>760</v>
+      </c>
+      <c r="T81" t="s">
         <v>463</v>
       </c>
-      <c r="L81" t="s">
-        <v>455</v>
-      </c>
-      <c r="M81" t="s">
-        <v>454</v>
-      </c>
-      <c r="N81" t="s">
+      <c r="U81" t="s">
         <v>464</v>
       </c>
-      <c r="O81" t="s">
-        <v>463</v>
-      </c>
-      <c r="P81" t="s">
-        <v>457</v>
-      </c>
-      <c r="Q81" t="s">
-        <v>463</v>
-      </c>
-      <c r="S81" t="s">
-        <v>762</v>
-      </c>
-      <c r="T81" t="s">
+      <c r="V81" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="82" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="U81" t="s">
+      <c r="S82" t="s">
         <v>466</v>
       </c>
-      <c r="V81" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A82" s="1" t="s">
+      <c r="T82" t="s">
         <v>467</v>
       </c>
-      <c r="S82" t="s">
+      <c r="U82" t="s">
         <v>468</v>
       </c>
-      <c r="T82" t="s">
+    </row>
+    <row r="83" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="U82" t="s">
+      <c r="S83" s="7" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A83" s="1" t="s">
+    <row r="84" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="S83" s="7" t="s">
+      <c r="B84" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A84" s="1" t="s">
+      <c r="C84" t="s">
+        <v>472</v>
+      </c>
+      <c r="D84" t="s">
+        <v>472</v>
+      </c>
+      <c r="E84" t="s">
+        <v>472</v>
+      </c>
+      <c r="F84" t="s">
         <v>473</v>
       </c>
-      <c r="B84" t="s">
+      <c r="G84" t="s">
         <v>474</v>
       </c>
-      <c r="C84" t="s">
-        <v>474</v>
-      </c>
-      <c r="D84" t="s">
-        <v>474</v>
-      </c>
-      <c r="E84" t="s">
-        <v>474</v>
-      </c>
-      <c r="F84" t="s">
+      <c r="H84" t="s">
         <v>475</v>
       </c>
-      <c r="G84" t="s">
+      <c r="I84" t="s">
         <v>476</v>
       </c>
-      <c r="H84" t="s">
+      <c r="S84" t="s">
         <v>477</v>
       </c>
-      <c r="I84" t="s">
+      <c r="T84" t="s">
+        <v>472</v>
+      </c>
+      <c r="U84" t="s">
+        <v>472</v>
+      </c>
+      <c r="V84" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="85" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="S84" t="s">
+      <c r="H85" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="T84" t="s">
-        <v>474</v>
-      </c>
-      <c r="U84" t="s">
-        <v>474</v>
-      </c>
-      <c r="V84" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A85" s="1" t="s">
+      <c r="S85" t="s">
         <v>480</v>
       </c>
-      <c r="H85" s="2" t="s">
+      <c r="T85" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="S85" t="s">
+      <c r="U85" t="s">
         <v>482</v>
       </c>
-      <c r="T85" s="2" t="s">
+    </row>
+    <row r="86" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="U85" t="s">
+      <c r="E86" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A86" s="1" t="s">
+      <c r="H86" t="s">
         <v>485</v>
       </c>
-      <c r="E86" t="s">
+      <c r="S86" t="s">
         <v>486</v>
       </c>
-      <c r="H86" t="s">
+      <c r="T86" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="S86" t="s">
+      <c r="U86" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="87" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="T86" s="2" t="s">
+      <c r="S87" t="s">
         <v>489</v>
       </c>
-      <c r="U86" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A87" s="1" t="s">
+    </row>
+    <row r="88" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="S87" t="s">
+      <c r="S88" s="21" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A88" s="1" t="s">
+    <row r="89" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="S88" s="21" t="s">
+      <c r="S89" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A89" s="1" t="s">
+    <row r="90" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
         <v>494</v>
       </c>
-      <c r="S89" t="s">
+      <c r="B90" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A90" s="3" t="s">
+      <c r="C90" t="s">
         <v>496</v>
       </c>
-      <c r="B90" t="s">
+      <c r="D90" t="s">
         <v>497</v>
       </c>
-      <c r="C90" t="s">
+      <c r="E90" t="s">
         <v>498</v>
       </c>
-      <c r="D90" t="s">
+      <c r="F90" t="s">
         <v>499</v>
       </c>
-      <c r="E90" t="s">
+      <c r="G90" t="s">
         <v>500</v>
       </c>
-      <c r="F90" t="s">
+      <c r="H90" t="s">
         <v>501</v>
       </c>
-      <c r="G90" t="s">
+      <c r="I90" t="s">
         <v>502</v>
       </c>
-      <c r="H90" t="s">
+      <c r="J90" t="s">
         <v>503</v>
       </c>
-      <c r="I90" t="s">
+      <c r="K90" t="s">
         <v>504</v>
       </c>
-      <c r="J90" t="s">
+      <c r="L90" t="s">
         <v>505</v>
       </c>
-      <c r="K90" t="s">
+      <c r="M90" t="s">
         <v>506</v>
       </c>
-      <c r="L90" t="s">
+      <c r="N90" t="s">
         <v>507</v>
       </c>
-      <c r="M90" t="s">
+      <c r="O90" t="s">
         <v>508</v>
       </c>
-      <c r="N90" t="s">
+      <c r="P90" t="s">
+        <v>510</v>
+      </c>
+      <c r="Q90" t="s">
         <v>509</v>
       </c>
-      <c r="O90" t="s">
-        <v>510</v>
-      </c>
-      <c r="P90" t="s">
+      <c r="S90" t="s">
+        <v>511</v>
+      </c>
+      <c r="T90" t="s">
         <v>512</v>
       </c>
-      <c r="Q90" t="s">
-        <v>511</v>
-      </c>
-      <c r="S90" t="s">
+      <c r="U90" t="s">
         <v>513</v>
       </c>
-      <c r="T90" t="s">
+    </row>
+    <row r="91" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
         <v>514</v>
       </c>
-      <c r="U90" t="s">
+      <c r="B91" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A91" s="3" t="s">
+      <c r="C91" t="s">
         <v>516</v>
       </c>
-      <c r="B91" t="s">
+      <c r="D91" t="s">
         <v>517</v>
       </c>
-      <c r="C91" t="s">
+      <c r="E91" t="s">
         <v>518</v>
       </c>
-      <c r="D91" t="s">
+      <c r="F91" t="s">
         <v>519</v>
       </c>
-      <c r="E91" t="s">
+      <c r="G91" t="s">
         <v>520</v>
       </c>
-      <c r="F91" t="s">
+      <c r="H91" t="s">
         <v>521</v>
       </c>
-      <c r="G91" t="s">
+      <c r="I91" t="s">
         <v>522</v>
       </c>
-      <c r="H91" t="s">
+      <c r="J91" t="s">
         <v>523</v>
       </c>
-      <c r="I91" t="s">
+      <c r="K91" t="s">
         <v>524</v>
       </c>
-      <c r="J91" t="s">
+      <c r="L91" t="s">
         <v>525</v>
       </c>
-      <c r="K91" t="s">
+      <c r="M91" t="s">
         <v>526</v>
       </c>
-      <c r="L91" t="s">
+      <c r="N91" t="s">
         <v>527</v>
       </c>
-      <c r="M91" t="s">
+      <c r="O91" t="s">
         <v>528</v>
       </c>
-      <c r="N91" t="s">
+      <c r="P91" t="s">
+        <v>530</v>
+      </c>
+      <c r="Q91" t="s">
         <v>529</v>
       </c>
-      <c r="O91" t="s">
-        <v>530</v>
-      </c>
-      <c r="P91" t="s">
+      <c r="S91" t="s">
+        <v>531</v>
+      </c>
+      <c r="T91" t="s">
         <v>532</v>
       </c>
-      <c r="Q91" t="s">
-        <v>531</v>
-      </c>
-      <c r="S91" t="s">
+      <c r="U91" t="s">
         <v>533</v>
       </c>
-      <c r="T91" t="s">
+    </row>
+    <row r="92" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
         <v>534</v>
       </c>
-      <c r="U91" t="s">
+      <c r="B92" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A92" s="3" t="s">
+      <c r="C92" t="s">
         <v>536</v>
       </c>
-      <c r="B92" t="s">
+      <c r="D92" t="s">
         <v>537</v>
       </c>
-      <c r="C92" t="s">
+      <c r="E92" t="s">
         <v>538</v>
       </c>
-      <c r="D92" t="s">
+      <c r="F92" t="s">
         <v>539</v>
       </c>
-      <c r="E92" t="s">
+      <c r="G92" t="s">
         <v>540</v>
       </c>
-      <c r="F92" t="s">
+      <c r="H92" t="s">
         <v>541</v>
       </c>
-      <c r="G92" t="s">
+      <c r="I92" t="s">
         <v>542</v>
       </c>
-      <c r="H92" t="s">
+      <c r="J92" t="s">
         <v>543</v>
       </c>
-      <c r="I92" t="s">
+      <c r="K92" t="s">
         <v>544</v>
       </c>
-      <c r="J92" t="s">
+      <c r="L92" t="s">
         <v>545</v>
       </c>
-      <c r="K92" t="s">
+      <c r="M92" t="s">
         <v>546</v>
       </c>
-      <c r="L92" t="s">
+      <c r="N92" t="s">
         <v>547</v>
       </c>
-      <c r="M92" t="s">
+      <c r="O92" t="s">
+        <v>528</v>
+      </c>
+      <c r="P92" t="s">
+        <v>549</v>
+      </c>
+      <c r="Q92" t="s">
         <v>548</v>
       </c>
-      <c r="N92" t="s">
-        <v>549</v>
-      </c>
-      <c r="O92" t="s">
-        <v>530</v>
-      </c>
-      <c r="P92" t="s">
+      <c r="S92" t="s">
+        <v>550</v>
+      </c>
+      <c r="T92" t="s">
         <v>551</v>
       </c>
-      <c r="Q92" t="s">
-        <v>550</v>
-      </c>
-      <c r="S92" t="s">
+      <c r="U92" t="s">
         <v>552</v>
       </c>
-      <c r="T92" t="s">
+    </row>
+    <row r="93" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="U92" t="s">
+      <c r="B93" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A93" s="3" t="s">
+      <c r="C93" t="s">
         <v>555</v>
       </c>
-      <c r="B93" t="s">
+      <c r="D93" t="s">
         <v>556</v>
       </c>
-      <c r="C93" t="s">
+      <c r="E93" t="s">
         <v>557</v>
       </c>
-      <c r="D93" t="s">
+      <c r="F93" t="s">
         <v>558</v>
       </c>
-      <c r="E93" t="s">
+      <c r="G93" t="s">
         <v>559</v>
       </c>
-      <c r="F93" t="s">
+      <c r="H93" t="s">
         <v>560</v>
       </c>
-      <c r="G93" t="s">
+      <c r="I93" t="s">
         <v>561</v>
       </c>
-      <c r="H93" t="s">
+      <c r="J93" t="s">
         <v>562</v>
       </c>
-      <c r="I93" t="s">
+      <c r="K93" t="s">
         <v>563</v>
       </c>
-      <c r="J93" t="s">
+      <c r="L93" t="s">
         <v>564</v>
       </c>
-      <c r="K93" t="s">
+      <c r="M93" t="s">
         <v>565</v>
       </c>
-      <c r="L93" t="s">
+      <c r="N93" t="s">
         <v>566</v>
       </c>
-      <c r="M93" t="s">
+      <c r="O93" t="s">
         <v>567</v>
       </c>
-      <c r="N93" t="s">
+      <c r="P93" t="s">
+        <v>569</v>
+      </c>
+      <c r="Q93" t="s">
         <v>568</v>
       </c>
-      <c r="O93" t="s">
-        <v>569</v>
-      </c>
-      <c r="P93" t="s">
+      <c r="S93" s="22" t="s">
+        <v>570</v>
+      </c>
+      <c r="T93" t="s">
         <v>571</v>
       </c>
-      <c r="Q93" t="s">
-        <v>570</v>
-      </c>
-      <c r="S93" s="22" t="s">
+      <c r="U93" t="s">
         <v>572</v>
       </c>
-      <c r="T93" t="s">
+    </row>
+    <row r="94" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
         <v>573</v>
       </c>
-      <c r="U93" t="s">
+      <c r="B94" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A94" s="3" t="s">
+      <c r="C94" t="s">
         <v>575</v>
       </c>
-      <c r="B94" t="s">
+      <c r="D94" t="s">
         <v>576</v>
       </c>
-      <c r="C94" t="s">
+      <c r="E94" t="s">
         <v>577</v>
       </c>
-      <c r="D94" t="s">
+      <c r="F94" t="s">
         <v>578</v>
       </c>
-      <c r="E94" t="s">
+      <c r="G94" t="s">
         <v>579</v>
       </c>
-      <c r="F94" t="s">
+      <c r="H94" t="s">
         <v>580</v>
       </c>
-      <c r="G94" t="s">
+      <c r="I94" t="s">
         <v>581</v>
       </c>
-      <c r="H94" t="s">
+      <c r="J94" t="s">
         <v>582</v>
       </c>
-      <c r="I94" t="s">
+      <c r="K94" t="s">
         <v>583</v>
       </c>
-      <c r="J94" t="s">
+      <c r="L94" t="s">
         <v>584</v>
       </c>
-      <c r="K94" t="s">
+      <c r="M94" t="s">
         <v>585</v>
       </c>
-      <c r="L94" t="s">
+      <c r="O94" t="s">
         <v>586</v>
       </c>
-      <c r="M94" t="s">
+      <c r="P94" t="s">
+        <v>588</v>
+      </c>
+      <c r="Q94" t="s">
         <v>587</v>
       </c>
-      <c r="O94" t="s">
-        <v>588</v>
-      </c>
-      <c r="P94" t="s">
+      <c r="U94" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="95" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="Q94" t="s">
-        <v>589</v>
-      </c>
-      <c r="U94" t="s">
+      <c r="B95" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A95" s="3" t="s">
+      <c r="C95" t="s">
         <v>592</v>
       </c>
-      <c r="B95" t="s">
+      <c r="D95" t="s">
         <v>593</v>
       </c>
-      <c r="C95" t="s">
+      <c r="E95" t="s">
         <v>594</v>
       </c>
-      <c r="D95" t="s">
+      <c r="G95" t="s">
         <v>595</v>
       </c>
-      <c r="E95" t="s">
+      <c r="H95" t="s">
         <v>596</v>
       </c>
-      <c r="G95" t="s">
+      <c r="I95" t="s">
         <v>597</v>
       </c>
-      <c r="H95" t="s">
+      <c r="K95" t="s">
         <v>598</v>
       </c>
-      <c r="I95" t="s">
+      <c r="L95" t="s">
         <v>599</v>
       </c>
-      <c r="K95" t="s">
+      <c r="M95" t="s">
         <v>600</v>
       </c>
-      <c r="L95" t="s">
+      <c r="P95" t="s">
         <v>601</v>
       </c>
-      <c r="M95" t="s">
+      <c r="U95" t="s">
         <v>602</v>
       </c>
-      <c r="P95" t="s">
+    </row>
+    <row r="96" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
         <v>603</v>
       </c>
-      <c r="U95" t="s">
+      <c r="B96" t="s">
         <v>604</v>
       </c>
-    </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A96" s="3" t="s">
+      <c r="D96" t="s">
         <v>605</v>
       </c>
-      <c r="B96" t="s">
+      <c r="G96" t="s">
         <v>606</v>
       </c>
-      <c r="D96" t="s">
+      <c r="H96" t="s">
         <v>607</v>
       </c>
-      <c r="G96" t="s">
+      <c r="I96" t="s">
         <v>608</v>
       </c>
-      <c r="H96" t="s">
+      <c r="L96" t="s">
         <v>609</v>
       </c>
-      <c r="I96" t="s">
+      <c r="P96" t="s">
         <v>610</v>
       </c>
-      <c r="L96" t="s">
+    </row>
+    <row r="97" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
         <v>611</v>
       </c>
-      <c r="P96" t="s">
+      <c r="D97" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A97" s="3" t="s">
+      <c r="G97" t="s">
         <v>613</v>
       </c>
-      <c r="D97" t="s">
+      <c r="H97" t="s">
         <v>614</v>
       </c>
-      <c r="G97" t="s">
+      <c r="P97" t="s">
         <v>615</v>
       </c>
-      <c r="H97" t="s">
+    </row>
+    <row r="98" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
         <v>616</v>
       </c>
-      <c r="P97" t="s">
+      <c r="D98" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A98" s="3" t="s">
+      <c r="H98" t="s">
         <v>618</v>
       </c>
-      <c r="D98" t="s">
+    </row>
+    <row r="99" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="H98" t="s">
+      <c r="D99" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A99" s="3" t="s">
+      <c r="H99" t="s">
+        <v>559</v>
+      </c>
+      <c r="I99" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="100" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
         <v>621</v>
       </c>
-      <c r="D99" t="s">
+      <c r="S100" t="s">
         <v>622</v>
       </c>
-      <c r="H99" t="s">
-        <v>561</v>
-      </c>
-      <c r="I99" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A100" s="3" t="s">
+    </row>
+    <row r="101" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
         <v>623</v>
       </c>
-      <c r="S100" t="s">
+      <c r="S101" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A101" s="3" t="s">
+    <row r="102" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
         <v>625</v>
       </c>
-      <c r="S101" t="s">
+      <c r="S102" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A102" s="3" t="s">
+    <row r="103" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
         <v>627</v>
       </c>
-      <c r="S102" t="s">
+      <c r="B103" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A103" s="3" t="s">
+      <c r="C103" t="s">
+        <v>628</v>
+      </c>
+      <c r="D103" t="s">
+        <v>628</v>
+      </c>
+      <c r="E103" t="s">
+        <v>628</v>
+      </c>
+      <c r="F103" t="s">
+        <v>628</v>
+      </c>
+      <c r="H103" t="s">
+        <v>628</v>
+      </c>
+      <c r="I103" t="s">
+        <v>628</v>
+      </c>
+      <c r="J103" t="s">
+        <v>628</v>
+      </c>
+      <c r="M103" t="s">
         <v>629</v>
       </c>
-      <c r="B103" t="s">
+      <c r="S103" t="s">
         <v>630</v>
       </c>
-      <c r="C103" t="s">
-        <v>630</v>
-      </c>
-      <c r="D103" t="s">
-        <v>630</v>
-      </c>
-      <c r="E103" t="s">
-        <v>630</v>
-      </c>
-      <c r="F103" t="s">
-        <v>630</v>
-      </c>
-      <c r="H103" t="s">
-        <v>630</v>
-      </c>
-      <c r="I103" t="s">
-        <v>630</v>
-      </c>
-      <c r="J103" t="s">
-        <v>630</v>
-      </c>
-      <c r="M103" t="s">
+      <c r="T103" t="s">
+        <v>628</v>
+      </c>
+      <c r="U103" t="s">
+        <v>628</v>
+      </c>
+      <c r="V103" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="104" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A104" s="7" t="s">
         <v>631</v>
       </c>
-      <c r="S103" t="s">
+      <c r="B104" t="s">
         <v>632</v>
       </c>
-      <c r="T103" t="s">
-        <v>630</v>
-      </c>
-      <c r="U103" t="s">
-        <v>630</v>
-      </c>
-      <c r="V103" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A104" s="7" t="s">
+      <c r="C104" t="s">
+        <v>632</v>
+      </c>
+      <c r="D104" t="s">
+        <v>632</v>
+      </c>
+      <c r="E104" t="s">
+        <v>632</v>
+      </c>
+      <c r="F104" t="s">
+        <v>632</v>
+      </c>
+      <c r="G104" t="s">
+        <v>632</v>
+      </c>
+      <c r="H104" t="s">
+        <v>632</v>
+      </c>
+      <c r="I104" t="s">
+        <v>632</v>
+      </c>
+      <c r="J104" t="s">
+        <v>632</v>
+      </c>
+      <c r="K104" t="s">
+        <v>632</v>
+      </c>
+      <c r="L104" t="s">
+        <v>632</v>
+      </c>
+      <c r="M104" t="s">
+        <v>632</v>
+      </c>
+      <c r="N104" t="s">
+        <v>632</v>
+      </c>
+      <c r="O104" t="s">
+        <v>632</v>
+      </c>
+      <c r="P104" t="s">
+        <v>632</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>632</v>
+      </c>
+      <c r="R104" t="s">
+        <v>632</v>
+      </c>
+      <c r="S104" t="s">
         <v>633</v>
       </c>
-      <c r="B104" t="s">
+      <c r="T104" t="s">
+        <v>632</v>
+      </c>
+      <c r="U104" t="s">
+        <v>632</v>
+      </c>
+      <c r="V104" t="s">
+        <v>632</v>
+      </c>
+      <c r="W104" t="s">
+        <v>632</v>
+      </c>
+      <c r="X104" t="s">
+        <v>632</v>
+      </c>
+      <c r="Y104" t="s">
+        <v>632</v>
+      </c>
+      <c r="Z104" t="s">
+        <v>632</v>
+      </c>
+      <c r="AA104" t="s">
+        <v>632</v>
+      </c>
+      <c r="AB104" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="105" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A105" s="7" t="s">
+        <v>639</v>
+      </c>
+      <c r="B105" t="s">
+        <v>635</v>
+      </c>
+      <c r="C105" t="s">
+        <v>635</v>
+      </c>
+      <c r="D105" t="s">
+        <v>635</v>
+      </c>
+      <c r="E105" t="s">
+        <v>635</v>
+      </c>
+      <c r="F105" t="s">
+        <v>635</v>
+      </c>
+      <c r="G105" t="s">
+        <v>635</v>
+      </c>
+      <c r="H105" t="s">
+        <v>635</v>
+      </c>
+      <c r="I105" t="s">
+        <v>635</v>
+      </c>
+      <c r="J105" t="s">
+        <v>635</v>
+      </c>
+      <c r="K105" t="s">
+        <v>635</v>
+      </c>
+      <c r="L105" t="s">
+        <v>635</v>
+      </c>
+      <c r="M105" t="s">
+        <v>635</v>
+      </c>
+      <c r="N105" t="s">
+        <v>635</v>
+      </c>
+      <c r="O105" t="s">
+        <v>635</v>
+      </c>
+      <c r="P105" t="s">
+        <v>635</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>635</v>
+      </c>
+      <c r="R105" t="s">
+        <v>635</v>
+      </c>
+      <c r="S105" t="s">
+        <v>636</v>
+      </c>
+      <c r="T105" t="s">
+        <v>635</v>
+      </c>
+      <c r="U105" t="s">
+        <v>635</v>
+      </c>
+      <c r="V105" t="s">
+        <v>635</v>
+      </c>
+      <c r="W105" t="s">
+        <v>635</v>
+      </c>
+      <c r="X105" t="s">
+        <v>635</v>
+      </c>
+      <c r="Y105" t="s">
+        <v>635</v>
+      </c>
+      <c r="Z105" t="s">
+        <v>635</v>
+      </c>
+      <c r="AA105" t="s">
+        <v>635</v>
+      </c>
+      <c r="AB105" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="106" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A106" s="7" t="s">
         <v>634</v>
-      </c>
-      <c r="C104" t="s">
-        <v>634</v>
-      </c>
-      <c r="D104" t="s">
-        <v>634</v>
-      </c>
-      <c r="E104" t="s">
-        <v>634</v>
-      </c>
-      <c r="F104" t="s">
-        <v>634</v>
-      </c>
-      <c r="G104" t="s">
-        <v>634</v>
-      </c>
-      <c r="H104" t="s">
-        <v>634</v>
-      </c>
-      <c r="I104" t="s">
-        <v>634</v>
-      </c>
-      <c r="J104" t="s">
-        <v>634</v>
-      </c>
-      <c r="K104" t="s">
-        <v>634</v>
-      </c>
-      <c r="Q104" t="s">
-        <v>634</v>
-      </c>
-      <c r="S104" t="s">
-        <v>635</v>
-      </c>
-      <c r="T104" t="s">
-        <v>634</v>
-      </c>
-      <c r="U104" t="s">
-        <v>634</v>
-      </c>
-      <c r="V104" t="s">
-        <v>634</v>
-      </c>
-      <c r="X104" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A105" s="7" t="s">
-        <v>636</v>
-      </c>
-      <c r="B105" t="s">
-        <v>637</v>
-      </c>
-      <c r="C105" t="s">
-        <v>637</v>
-      </c>
-      <c r="D105" t="s">
-        <v>637</v>
-      </c>
-      <c r="E105" t="s">
-        <v>637</v>
-      </c>
-      <c r="F105" t="s">
-        <v>637</v>
-      </c>
-      <c r="G105" t="s">
-        <v>637</v>
-      </c>
-      <c r="H105" t="s">
-        <v>637</v>
-      </c>
-      <c r="I105" t="s">
-        <v>637</v>
-      </c>
-      <c r="J105" t="s">
-        <v>637</v>
-      </c>
-      <c r="K105" t="s">
-        <v>637</v>
-      </c>
-      <c r="Q105" t="s">
-        <v>637</v>
-      </c>
-      <c r="S105" t="s">
-        <v>638</v>
-      </c>
-      <c r="T105" t="s">
-        <v>637</v>
-      </c>
-      <c r="U105" t="s">
-        <v>637</v>
-      </c>
-      <c r="V105" t="s">
-        <v>637</v>
-      </c>
-      <c r="X105" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A106" s="7" t="s">
-        <v>639</v>
       </c>
       <c r="B106" t="s">
         <v>640</v>
       </c>
-      <c r="C106" t="s">
-        <v>640</v>
-      </c>
       <c r="D106" t="s">
         <v>640</v>
       </c>
       <c r="E106" t="s">
         <v>640</v>
       </c>
+      <c r="K106" t="s">
+        <v>640</v>
+      </c>
+      <c r="L106" t="s">
+        <v>640</v>
+      </c>
+      <c r="M106" t="s">
+        <v>640</v>
+      </c>
+      <c r="O106" t="s">
+        <v>640</v>
+      </c>
+      <c r="P106" t="s">
+        <v>640</v>
+      </c>
+      <c r="S106" t="s">
+        <v>641</v>
+      </c>
       <c r="T106" t="s">
         <v>640</v>
       </c>
@@ -8910,390 +9088,402 @@
       <c r="X106" t="s">
         <v>640</v>
       </c>
-    </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Z106" t="s">
+        <v>640</v>
+      </c>
+      <c r="AB106" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="107" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A107" s="7" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B107" t="s">
+        <v>638</v>
+      </c>
+      <c r="C107" t="s">
+        <v>638</v>
+      </c>
+      <c r="D107" t="s">
+        <v>638</v>
+      </c>
+      <c r="E107" t="s">
+        <v>638</v>
+      </c>
+      <c r="L107" t="s">
+        <v>638</v>
+      </c>
+      <c r="O107" t="s">
+        <v>638</v>
+      </c>
+      <c r="T107" t="s">
+        <v>638</v>
+      </c>
+      <c r="U107" t="s">
+        <v>638</v>
+      </c>
+      <c r="V107" t="s">
+        <v>638</v>
+      </c>
+      <c r="X107" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="108" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A108" s="7" t="s">
         <v>642</v>
       </c>
-      <c r="D107" t="s">
-        <v>642</v>
-      </c>
-      <c r="E107" t="s">
-        <v>642</v>
-      </c>
-      <c r="K107" t="s">
-        <v>642</v>
-      </c>
-      <c r="S107" t="s">
+      <c r="B108" s="7" t="s">
+        <v>639</v>
+      </c>
+      <c r="C108" t="s">
         <v>643</v>
       </c>
-      <c r="T107" t="s">
-        <v>642</v>
-      </c>
-      <c r="U107" t="s">
-        <v>642</v>
-      </c>
-      <c r="V107" t="s">
-        <v>642</v>
-      </c>
-      <c r="X107" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A108" s="7" t="s">
+      <c r="G108" t="s">
         <v>644</v>
       </c>
-      <c r="C108" t="s">
+      <c r="J108" t="s">
         <v>645</v>
       </c>
-      <c r="G108" t="s">
+    </row>
+    <row r="109" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A109" s="3" t="s">
         <v>646</v>
       </c>
-      <c r="J108" t="s">
+      <c r="S109" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A109" s="3" t="s">
+      <c r="T109" t="s">
         <v>648</v>
       </c>
-      <c r="S109" t="s">
+      <c r="U109" t="s">
         <v>649</v>
       </c>
-      <c r="T109" t="s">
+    </row>
+    <row r="110" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
         <v>650</v>
       </c>
-      <c r="U109" t="s">
+      <c r="S110" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A110" s="3" t="s">
+      <c r="T110" t="s">
         <v>652</v>
       </c>
-      <c r="S110" t="s">
+      <c r="U110" t="s">
         <v>653</v>
       </c>
-      <c r="T110" t="s">
+    </row>
+    <row r="111" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
         <v>654</v>
       </c>
-      <c r="U110" t="s">
+      <c r="S111" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A111" s="3" t="s">
+      <c r="T111" t="s">
         <v>656</v>
       </c>
-      <c r="S111" t="s">
+      <c r="U111" t="s">
         <v>657</v>
       </c>
-      <c r="T111" t="s">
+    </row>
+    <row r="112" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
         <v>658</v>
       </c>
-      <c r="U111" t="s">
+      <c r="U112" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A112" s="3" t="s">
+    <row r="113" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
         <v>660</v>
       </c>
-      <c r="U112" t="s">
+      <c r="S113" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A113" s="3" t="s">
+    <row r="114" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
         <v>662</v>
       </c>
-      <c r="S113" t="s">
+      <c r="S114" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A114" s="3" t="s">
+      <c r="T114" s="23" t="s">
         <v>664</v>
       </c>
-      <c r="S114" t="s">
+      <c r="U114" t="s">
         <v>665</v>
       </c>
-      <c r="T114" s="23" t="s">
+    </row>
+    <row r="115" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A115" s="3" t="s">
         <v>666</v>
       </c>
-      <c r="U114" t="s">
+      <c r="S115" t="s">
         <v>667</v>
       </c>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A115" s="3" t="s">
+    <row r="116" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A116" s="3" t="s">
         <v>668</v>
       </c>
-      <c r="S115" t="s">
+      <c r="U116" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A116" s="3" t="s">
+    <row r="117" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A117" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="B117" t="s">
+        <v>793</v>
+      </c>
+      <c r="C117" t="s">
+        <v>799</v>
+      </c>
+      <c r="D117" t="s">
+        <v>801</v>
+      </c>
+      <c r="E117" t="s">
+        <v>803</v>
+      </c>
+      <c r="F117" t="s">
+        <v>795</v>
+      </c>
+      <c r="G117" t="s">
+        <v>787</v>
+      </c>
+      <c r="H117" t="s">
+        <v>791</v>
+      </c>
+      <c r="J117" t="s">
+        <v>805</v>
+      </c>
+      <c r="K117" t="s">
+        <v>797</v>
+      </c>
+      <c r="L117" t="s">
+        <v>782</v>
+      </c>
+      <c r="O117" t="s">
+        <v>833</v>
+      </c>
+      <c r="P117" t="s">
+        <v>784</v>
+      </c>
+      <c r="S117" t="s">
+        <v>705</v>
+      </c>
+      <c r="T117" t="s">
+        <v>706</v>
+      </c>
+      <c r="U117" t="s">
+        <v>707</v>
+      </c>
+      <c r="V117" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="118" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A118" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="B118" t="s">
+        <v>792</v>
+      </c>
+      <c r="C118" t="s">
+        <v>798</v>
+      </c>
+      <c r="D118" t="s">
+        <v>800</v>
+      </c>
+      <c r="E118" t="s">
+        <v>802</v>
+      </c>
+      <c r="F118" t="s">
+        <v>794</v>
+      </c>
+      <c r="G118" t="s">
+        <v>786</v>
+      </c>
+      <c r="H118" t="s">
+        <v>790</v>
+      </c>
+      <c r="J118" t="s">
+        <v>804</v>
+      </c>
+      <c r="K118" t="s">
+        <v>796</v>
+      </c>
+      <c r="L118" t="s">
+        <v>783</v>
+      </c>
+      <c r="O118" t="s">
+        <v>822</v>
+      </c>
+      <c r="P118" t="s">
+        <v>785</v>
+      </c>
+      <c r="S118" t="s">
+        <v>701</v>
+      </c>
+      <c r="T118" t="s">
+        <v>702</v>
+      </c>
+      <c r="U118" t="s">
+        <v>703</v>
+      </c>
+      <c r="V118" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="119" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A119" s="3" t="s">
+        <v>750</v>
+      </c>
+      <c r="B119" s="9" t="s">
+        <v>758</v>
+      </c>
+      <c r="C119" t="s">
+        <v>757</v>
+      </c>
+      <c r="G119" s="9" t="s">
+        <v>756</v>
+      </c>
+      <c r="H119" t="s">
+        <v>755</v>
+      </c>
+      <c r="K119" s="9" t="s">
+        <v>754</v>
+      </c>
+      <c r="M119" s="9" t="s">
+        <v>753</v>
+      </c>
+      <c r="N119" t="s">
+        <v>751</v>
+      </c>
+      <c r="O119" t="s">
+        <v>752</v>
+      </c>
+      <c r="V119" s="9" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="120" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A120" s="3" t="s">
         <v>670</v>
       </c>
-      <c r="U116" t="s">
+      <c r="B120" t="s">
+        <v>672</v>
+      </c>
+      <c r="C120" t="s">
+        <v>673</v>
+      </c>
+      <c r="D120" t="s">
+        <v>674</v>
+      </c>
+      <c r="E120" t="s">
+        <v>675</v>
+      </c>
+      <c r="F120" t="s">
+        <v>676</v>
+      </c>
+      <c r="H120" t="s">
+        <v>677</v>
+      </c>
+      <c r="I120" t="s">
+        <v>678</v>
+      </c>
+      <c r="J120" s="24" t="s">
+        <v>679</v>
+      </c>
+      <c r="K120" t="s">
+        <v>767</v>
+      </c>
+      <c r="L120" t="s">
+        <v>843</v>
+      </c>
+      <c r="M120" t="s">
+        <v>778</v>
+      </c>
+      <c r="N120" t="s">
+        <v>763</v>
+      </c>
+      <c r="O120" t="s">
+        <v>769</v>
+      </c>
+      <c r="S120" t="s">
+        <v>680</v>
+      </c>
+      <c r="T120" t="s">
+        <v>681</v>
+      </c>
+      <c r="U120" t="s">
+        <v>682</v>
+      </c>
+      <c r="V120" t="s">
         <v>671</v>
       </c>
     </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A117" s="3" t="s">
-        <v>782</v>
-      </c>
-      <c r="B117" t="s">
-        <v>795</v>
-      </c>
-      <c r="C117" t="s">
-        <v>801</v>
-      </c>
-      <c r="D117" t="s">
-        <v>803</v>
-      </c>
-      <c r="E117" t="s">
-        <v>805</v>
-      </c>
-      <c r="F117" t="s">
-        <v>797</v>
-      </c>
-      <c r="G117" t="s">
-        <v>789</v>
-      </c>
-      <c r="H117" t="s">
-        <v>793</v>
-      </c>
-      <c r="J117" t="s">
-        <v>807</v>
-      </c>
-      <c r="K117" t="s">
-        <v>799</v>
-      </c>
-      <c r="L117" t="s">
-        <v>784</v>
-      </c>
-      <c r="O117" t="s">
-        <v>835</v>
-      </c>
-      <c r="P117" t="s">
-        <v>786</v>
-      </c>
-      <c r="S117" t="s">
-        <v>707</v>
-      </c>
-      <c r="T117" t="s">
-        <v>708</v>
-      </c>
-      <c r="U117" t="s">
-        <v>709</v>
-      </c>
-      <c r="V117" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A118" s="3" t="s">
-        <v>783</v>
-      </c>
-      <c r="B118" t="s">
-        <v>794</v>
-      </c>
-      <c r="C118" t="s">
-        <v>800</v>
-      </c>
-      <c r="D118" t="s">
-        <v>802</v>
-      </c>
-      <c r="E118" t="s">
-        <v>804</v>
-      </c>
-      <c r="F118" t="s">
-        <v>796</v>
-      </c>
-      <c r="G118" t="s">
-        <v>788</v>
-      </c>
-      <c r="H118" t="s">
-        <v>792</v>
-      </c>
-      <c r="J118" t="s">
-        <v>806</v>
-      </c>
-      <c r="K118" t="s">
-        <v>798</v>
-      </c>
-      <c r="L118" t="s">
-        <v>785</v>
-      </c>
-      <c r="O118" t="s">
-        <v>824</v>
-      </c>
-      <c r="P118" t="s">
-        <v>787</v>
-      </c>
-      <c r="S118" t="s">
-        <v>703</v>
-      </c>
-      <c r="T118" t="s">
-        <v>704</v>
-      </c>
-      <c r="U118" t="s">
-        <v>705</v>
-      </c>
-      <c r="V118" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A119" s="3" t="s">
-        <v>752</v>
-      </c>
-      <c r="B119" s="9" t="s">
-        <v>760</v>
-      </c>
-      <c r="C119" t="s">
-        <v>759</v>
-      </c>
-      <c r="G119" s="9" t="s">
-        <v>758</v>
-      </c>
-      <c r="H119" t="s">
-        <v>757</v>
-      </c>
-      <c r="K119" s="9" t="s">
-        <v>756</v>
-      </c>
-      <c r="M119" s="9" t="s">
-        <v>755</v>
-      </c>
-      <c r="N119" t="s">
-        <v>753</v>
-      </c>
-      <c r="O119" t="s">
-        <v>754</v>
-      </c>
-      <c r="V119" s="9" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A120" s="3" t="s">
-        <v>672</v>
-      </c>
-      <c r="B120" t="s">
-        <v>674</v>
-      </c>
-      <c r="C120" t="s">
-        <v>675</v>
-      </c>
-      <c r="D120" t="s">
-        <v>676</v>
-      </c>
-      <c r="E120" t="s">
-        <v>677</v>
-      </c>
-      <c r="F120" t="s">
-        <v>678</v>
-      </c>
-      <c r="H120" t="s">
-        <v>679</v>
-      </c>
-      <c r="I120" t="s">
-        <v>680</v>
-      </c>
-      <c r="J120" s="24" t="s">
-        <v>681</v>
-      </c>
-      <c r="K120" t="s">
-        <v>769</v>
-      </c>
-      <c r="L120" t="s">
-        <v>845</v>
-      </c>
-      <c r="M120" t="s">
-        <v>780</v>
-      </c>
-      <c r="N120" t="s">
-        <v>765</v>
-      </c>
-      <c r="O120" t="s">
-        <v>771</v>
-      </c>
-      <c r="S120" t="s">
-        <v>682</v>
-      </c>
-      <c r="T120" t="s">
+    <row r="121" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A121" s="3" t="s">
         <v>683</v>
       </c>
-      <c r="U120" t="s">
+      <c r="B121" t="s">
         <v>684</v>
       </c>
-      <c r="V120" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A121" s="3" t="s">
+      <c r="C121" t="s">
+        <v>762</v>
+      </c>
+      <c r="D121" t="s">
         <v>685</v>
       </c>
-      <c r="B121" t="s">
+      <c r="F121" t="s">
         <v>686</v>
       </c>
-      <c r="C121" t="s">
-        <v>764</v>
-      </c>
-      <c r="D121" t="s">
+      <c r="G121" t="s">
         <v>687</v>
       </c>
-      <c r="F121" t="s">
+      <c r="H121" t="s">
         <v>688</v>
       </c>
-      <c r="G121" t="s">
+      <c r="I121" t="s">
         <v>689</v>
       </c>
-      <c r="H121" t="s">
+      <c r="J121" t="s">
         <v>690</v>
       </c>
-      <c r="I121" t="s">
+      <c r="M121" t="s">
         <v>691</v>
       </c>
-      <c r="J121" t="s">
+      <c r="N121" t="s">
         <v>692</v>
       </c>
-      <c r="M121" t="s">
+      <c r="O121" t="s">
+        <v>768</v>
+      </c>
+      <c r="Q121" t="s">
         <v>693</v>
       </c>
-      <c r="N121" t="s">
+      <c r="T121" t="s">
         <v>694</v>
       </c>
-      <c r="O121" t="s">
-        <v>770</v>
-      </c>
-      <c r="Q121" t="s">
+    </row>
+    <row r="122" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A122" s="3" t="s">
         <v>695</v>
       </c>
-      <c r="T121" t="s">
+      <c r="S122" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A122" s="3" t="s">
+    <row r="123" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A123" s="3" t="s">
         <v>697</v>
-      </c>
-      <c r="S122" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A123" s="3" t="s">
-        <v>699</v>
       </c>
       <c r="B123">
         <v>10</v>
@@ -9320,9 +9510,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B124">
         <v>6300</v>
@@ -9352,9 +9542,9 @@
         <v>6300</v>
       </c>
     </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B125">
         <v>6500</v>
@@ -9414,218 +9604,218 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="S126" t="s">
+        <v>701</v>
+      </c>
+      <c r="T126" t="s">
         <v>702</v>
       </c>
-      <c r="S126" t="s">
+      <c r="U126" t="s">
         <v>703</v>
       </c>
-      <c r="T126" t="s">
+    </row>
+    <row r="127" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A127" s="3" t="s">
         <v>704</v>
       </c>
-      <c r="U126" t="s">
+      <c r="S127" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A127" s="3" t="s">
+      <c r="T127" t="s">
         <v>706</v>
       </c>
-      <c r="S127" t="s">
+      <c r="U127" t="s">
         <v>707</v>
       </c>
-      <c r="T127" t="s">
+    </row>
+    <row r="129" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A129" s="3" t="s">
         <v>708</v>
       </c>
-      <c r="U127" t="s">
+      <c r="B129" t="s">
+        <v>28</v>
+      </c>
+      <c r="C129" t="s">
+        <v>28</v>
+      </c>
+      <c r="D129" t="s">
+        <v>28</v>
+      </c>
+      <c r="E129" t="s">
+        <v>28</v>
+      </c>
+      <c r="F129" t="s">
+        <v>28</v>
+      </c>
+      <c r="G129" t="s">
+        <v>28</v>
+      </c>
+      <c r="H129" t="s">
+        <v>28</v>
+      </c>
+      <c r="I129" t="s">
+        <v>28</v>
+      </c>
+      <c r="J129" t="s">
+        <v>28</v>
+      </c>
+      <c r="V129" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="130" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A130" s="3" t="s">
         <v>709</v>
       </c>
-    </row>
-    <row r="129" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A129" s="3" t="s">
+      <c r="B130" t="s">
+        <v>28</v>
+      </c>
+      <c r="D130" t="s">
+        <v>28</v>
+      </c>
+      <c r="E130" t="s">
+        <v>28</v>
+      </c>
+      <c r="V130" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="131" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A131" s="3" t="s">
         <v>710</v>
       </c>
-      <c r="B129" t="s">
-        <v>28</v>
-      </c>
-      <c r="C129" t="s">
-        <v>28</v>
-      </c>
-      <c r="D129" t="s">
-        <v>28</v>
-      </c>
-      <c r="E129" t="s">
-        <v>28</v>
-      </c>
-      <c r="F129" t="s">
-        <v>28</v>
-      </c>
-      <c r="G129" t="s">
-        <v>28</v>
-      </c>
-      <c r="H129" t="s">
-        <v>28</v>
-      </c>
-      <c r="I129" t="s">
-        <v>28</v>
-      </c>
-      <c r="J129" t="s">
-        <v>28</v>
-      </c>
-      <c r="V129" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="130" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A130" s="3" t="s">
+      <c r="D131" t="s">
+        <v>812</v>
+      </c>
+      <c r="H131" t="s">
         <v>711</v>
       </c>
-      <c r="B130" t="s">
-        <v>28</v>
-      </c>
-      <c r="D130" t="s">
-        <v>28</v>
-      </c>
-      <c r="E130" t="s">
-        <v>28</v>
-      </c>
-      <c r="V130" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="131" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A131" s="3" t="s">
+      <c r="I131" t="s">
+        <v>840</v>
+      </c>
+      <c r="K131" t="s">
+        <v>813</v>
+      </c>
+      <c r="L131" t="s">
+        <v>823</v>
+      </c>
+      <c r="M131" t="s">
+        <v>813</v>
+      </c>
+      <c r="N131" t="s">
+        <v>813</v>
+      </c>
+      <c r="O131" t="s">
+        <v>813</v>
+      </c>
+      <c r="P131" t="s">
+        <v>823</v>
+      </c>
+      <c r="Q131" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="132" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A132" s="3" t="s">
         <v>712</v>
       </c>
-      <c r="D131" t="s">
-        <v>814</v>
-      </c>
-      <c r="H131" t="s">
+      <c r="G132" t="s">
+        <v>815</v>
+      </c>
+      <c r="M132" t="s">
+        <v>813</v>
+      </c>
+      <c r="N132" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="133" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A133" s="3" t="s">
         <v>713</v>
       </c>
-      <c r="I131" t="s">
-        <v>842</v>
-      </c>
-      <c r="K131" t="s">
-        <v>815</v>
-      </c>
-      <c r="L131" t="s">
-        <v>825</v>
-      </c>
-      <c r="M131" t="s">
-        <v>815</v>
-      </c>
-      <c r="N131" t="s">
-        <v>815</v>
-      </c>
-      <c r="O131" t="s">
-        <v>815</v>
-      </c>
-      <c r="P131" t="s">
-        <v>825</v>
-      </c>
-      <c r="Q131" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="132" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A132" s="3" t="s">
+      <c r="V133" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="134" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A134" s="3" t="s">
         <v>714</v>
       </c>
-      <c r="G132" t="s">
-        <v>817</v>
-      </c>
-      <c r="M132" t="s">
-        <v>815</v>
-      </c>
-      <c r="N132" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="133" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A133" s="3" t="s">
+    </row>
+    <row r="135" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A135" s="3" t="s">
         <v>715</v>
       </c>
-      <c r="V133" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="134" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A134" s="3" t="s">
+      <c r="L135" t="s">
+        <v>823</v>
+      </c>
+      <c r="M135" t="s">
+        <v>711</v>
+      </c>
+      <c r="N135" t="s">
+        <v>711</v>
+      </c>
+      <c r="O135" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q135" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="136" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A136" s="3" t="s">
         <v>716</v>
       </c>
-    </row>
-    <row r="135" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A135" s="3" t="s">
+      <c r="M136" t="s">
+        <v>711</v>
+      </c>
+      <c r="N136" t="s">
+        <v>711</v>
+      </c>
+      <c r="O136" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q136" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="137" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A137" s="3" t="s">
         <v>717</v>
       </c>
-      <c r="L135" t="s">
-        <v>825</v>
-      </c>
-      <c r="M135" t="s">
-        <v>713</v>
-      </c>
-      <c r="N135" t="s">
-        <v>713</v>
-      </c>
-      <c r="O135" t="s">
-        <v>713</v>
-      </c>
-      <c r="Q135" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="136" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A136" s="3" t="s">
+      <c r="I137" t="s">
+        <v>839</v>
+      </c>
+      <c r="M137" t="s">
+        <v>711</v>
+      </c>
+      <c r="N137" t="s">
+        <v>711</v>
+      </c>
+      <c r="O137" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q137" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="138" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A138" s="3" t="s">
         <v>718</v>
       </c>
-      <c r="M136" t="s">
-        <v>713</v>
-      </c>
-      <c r="N136" t="s">
-        <v>713</v>
-      </c>
-      <c r="O136" t="s">
-        <v>713</v>
-      </c>
-      <c r="Q136" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="137" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A137" s="3" t="s">
+    </row>
+    <row r="139" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A139" s="3" t="s">
         <v>719</v>
       </c>
-      <c r="I137" t="s">
-        <v>841</v>
-      </c>
-      <c r="M137" t="s">
-        <v>713</v>
-      </c>
-      <c r="N137" t="s">
-        <v>713</v>
-      </c>
-      <c r="O137" t="s">
-        <v>713</v>
-      </c>
-      <c r="Q137" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="138" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A138" s="3" t="s">
+    </row>
+    <row r="140" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A140" s="3" t="s">
         <v>720</v>
-      </c>
-    </row>
-    <row r="139" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A139" s="3" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="140" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A140" s="3" t="s">
-        <v>722</v>
       </c>
       <c r="B140" t="s">
         <v>43</v>
@@ -9655,9 +9845,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="141" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B141" t="s">
         <v>43</v>
@@ -9684,167 +9874,167 @@
         <v>43</v>
       </c>
     </row>
-    <row r="142" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
+        <v>722</v>
+      </c>
+      <c r="Q142" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="143" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A143" s="3" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="144" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A144" s="3" t="s">
         <v>724</v>
       </c>
-      <c r="Q142" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="143" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A143" s="3" t="s">
+      <c r="M144" t="s">
+        <v>711</v>
+      </c>
+      <c r="N144" t="s">
+        <v>711</v>
+      </c>
+      <c r="O144" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q144" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="145" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A145" s="3" t="s">
         <v>725</v>
       </c>
-    </row>
-    <row r="144" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A144" s="3" t="s">
+      <c r="M145" t="s">
+        <v>711</v>
+      </c>
+      <c r="N145" t="s">
+        <v>711</v>
+      </c>
+      <c r="O145" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q145" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="146" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A146" s="3" t="s">
         <v>726</v>
       </c>
-      <c r="M144" t="s">
-        <v>713</v>
-      </c>
-      <c r="N144" t="s">
-        <v>713</v>
-      </c>
-      <c r="O144" t="s">
-        <v>713</v>
-      </c>
-      <c r="Q144" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A145" s="3" t="s">
+    </row>
+    <row r="147" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A147" s="3" t="s">
         <v>727</v>
       </c>
-      <c r="M145" t="s">
-        <v>713</v>
-      </c>
-      <c r="N145" t="s">
-        <v>713</v>
-      </c>
-      <c r="O145" t="s">
-        <v>713</v>
-      </c>
-      <c r="Q145" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A146" s="3" t="s">
+    </row>
+    <row r="148" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A148" s="3" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A147" s="3" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A148" s="3" t="s">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A149" s="3" t="s">
+        <v>821</v>
+      </c>
+      <c r="M149" t="s">
+        <v>711</v>
+      </c>
+      <c r="N149" t="s">
+        <v>711</v>
+      </c>
+      <c r="O149" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="150" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A150" s="3" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A149" s="3" t="s">
-        <v>823</v>
-      </c>
-      <c r="M149" t="s">
-        <v>713</v>
-      </c>
-      <c r="N149" t="s">
-        <v>713</v>
-      </c>
-      <c r="O149" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A150" s="3" t="s">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A151" s="3" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="152" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A152" s="3" t="s">
+        <v>838</v>
+      </c>
+      <c r="M152" t="s">
+        <v>711</v>
+      </c>
+      <c r="N152" t="s">
+        <v>711</v>
+      </c>
+      <c r="O152" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="153" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A153" s="1" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A151" s="3" t="s">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A154" s="3" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A152" s="3" t="s">
-        <v>840</v>
-      </c>
-      <c r="M152" t="s">
-        <v>713</v>
-      </c>
-      <c r="N152" t="s">
-        <v>713</v>
-      </c>
-      <c r="O152" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A153" s="1" t="s">
+      <c r="M154" t="s">
+        <v>813</v>
+      </c>
+      <c r="N154" t="s">
+        <v>711</v>
+      </c>
+      <c r="O154" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="155" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A155" s="3" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A154" s="3" t="s">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A156" s="3" t="s">
         <v>735</v>
       </c>
-      <c r="M154" t="s">
-        <v>815</v>
-      </c>
-      <c r="N154" t="s">
-        <v>713</v>
-      </c>
-      <c r="O154" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A155" s="3" t="s">
+      <c r="M156" t="s">
+        <v>711</v>
+      </c>
+      <c r="N156" t="s">
+        <v>711</v>
+      </c>
+      <c r="O156" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q156" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="157" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A157" s="3" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A156" s="3" t="s">
+      <c r="M157" t="s">
+        <v>711</v>
+      </c>
+      <c r="N157" t="s">
+        <v>711</v>
+      </c>
+      <c r="O157" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q157" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="158" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A158" s="3" t="s">
         <v>737</v>
-      </c>
-      <c r="M156" t="s">
-        <v>713</v>
-      </c>
-      <c r="N156" t="s">
-        <v>713</v>
-      </c>
-      <c r="O156" t="s">
-        <v>713</v>
-      </c>
-      <c r="Q156" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A157" s="3" t="s">
-        <v>738</v>
-      </c>
-      <c r="M157" t="s">
-        <v>713</v>
-      </c>
-      <c r="N157" t="s">
-        <v>713</v>
-      </c>
-      <c r="O157" t="s">
-        <v>713</v>
-      </c>
-      <c r="Q157" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A158" s="3" t="s">
-        <v>739</v>
       </c>
       <c r="H158" t="s">
         <v>43</v>
@@ -9853,110 +10043,110 @@
         <v>43</v>
       </c>
       <c r="M158" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="N158" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="O158" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="Q158" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.35">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="159" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
+        <v>738</v>
+      </c>
+      <c r="M159" t="s">
+        <v>711</v>
+      </c>
+      <c r="N159" t="s">
+        <v>711</v>
+      </c>
+      <c r="O159" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q159" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="160" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A160" s="3" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="161" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A161" s="3" t="s">
         <v>740</v>
       </c>
-      <c r="M159" t="s">
-        <v>713</v>
-      </c>
-      <c r="N159" t="s">
-        <v>713</v>
-      </c>
-      <c r="O159" t="s">
-        <v>713</v>
-      </c>
-      <c r="Q159" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A160" s="3" t="s">
+    </row>
+    <row r="162" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A162" s="3" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="161" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A161" s="3" t="s">
+    <row r="163" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A163" s="3" t="s">
+        <v>770</v>
+      </c>
+      <c r="G163" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="164" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A164" s="1" t="s">
         <v>742</v>
-      </c>
-    </row>
-    <row r="162" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A162" s="3" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="163" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A163" s="3" t="s">
-        <v>772</v>
-      </c>
-      <c r="G163" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="164" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A164" s="1" t="s">
-        <v>744</v>
       </c>
       <c r="F164" s="1"/>
       <c r="G164" s="1"/>
       <c r="H164" s="1"/>
       <c r="I164" s="1"/>
       <c r="N164" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="165" spans="1:22" x14ac:dyDescent="0.35">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="165" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="166" spans="1:22" x14ac:dyDescent="0.35">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="166" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A166" s="3" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="H166" s="1"/>
       <c r="J166" s="1"/>
     </row>
-    <row r="167" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="V167" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="168" spans="1:22" x14ac:dyDescent="0.35">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="168" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="H168" s="1"/>
     </row>
-    <row r="169" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="170" spans="1:22" x14ac:dyDescent="0.35">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="170" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="C170" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="171" spans="1:22" x14ac:dyDescent="0.35">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="171" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A171" s="3"/>
     </row>
   </sheetData>

</xml_diff>